<commit_message>
01.10.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/October/Others/Allocation Sheet.xlsx
+++ b/October/Others/Allocation Sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="121">
   <si>
     <t>BL60</t>
   </si>
@@ -433,7 +433,10 @@
     <t>V99</t>
   </si>
   <si>
-    <t>Md Shohel Rana</t>
+    <t>L65j</t>
+  </si>
+  <si>
+    <t>Md Robiul Islam</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,12 +583,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -600,7 +597,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -616,12 +613,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,7 +797,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -886,11 +877,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -910,176 +901,185 @@
     <xf numFmtId="1" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1098,13 +1098,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>29158</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>181171</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1143,13 +1143,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>194390</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1264,13 +1264,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>147792</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>42755</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>288667</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>114587</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -1282,7 +1282,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="147792" y="11825180"/>
+          <a:off x="147792" y="12072830"/>
           <a:ext cx="6779800" cy="271857"/>
           <a:chOff x="249" y="249"/>
           <a:chExt cx="635" cy="292"/>
@@ -1481,7 +1481,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2581,7 +2581,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3027,7 +3027,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3098,7 +3098,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3172,7 +3172,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3243,7 +3243,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3903,10 +3903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:U57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O60"/>
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3929,50 +3929,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="62"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="56" t="s">
+      <c r="A1" s="71"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
       <c r="A3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="61"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="60"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="69"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
@@ -3980,948 +3980,946 @@
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
-      <c r="L3" s="57" t="s">
+      <c r="L3" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="M3" s="58"/>
-      <c r="N3" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="O3" s="60"/>
-    </row>
-    <row r="4" spans="1:15" ht="16.5" thickTop="1">
-      <c r="A4" s="44" t="s">
+      <c r="M3" s="67"/>
+      <c r="N3" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="O3" s="69"/>
+    </row>
+    <row r="4" spans="1:15" ht="19.5" customHeight="1" thickTop="1">
+      <c r="A4" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="44" t="s">
+      <c r="H4" s="98"/>
+      <c r="I4" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="L4" s="45" t="s">
+      <c r="L4" s="98" t="s">
         <v>80</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="M4" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="45" t="s">
+      <c r="N4" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="98" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A5" s="48" t="s">
-        <v>44</v>
+    <row r="5" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A5" s="44" t="s">
+        <v>95</v>
       </c>
       <c r="B5" s="37">
-        <v>800</v>
+        <v>780</v>
       </c>
       <c r="C5" s="38">
-        <v>875</v>
+        <v>840</v>
       </c>
       <c r="D5" s="38"/>
       <c r="E5" s="38"/>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
       <c r="H5" s="38"/>
-      <c r="I5" s="47" t="s">
-        <v>86</v>
+      <c r="I5" s="43" t="s">
+        <v>88</v>
       </c>
       <c r="J5" s="39">
-        <v>5470</v>
+        <v>2780</v>
       </c>
       <c r="K5" s="38">
-        <v>5890</v>
+        <v>2990</v>
       </c>
       <c r="L5" s="38"/>
       <c r="M5" s="38"/>
       <c r="N5" s="38"/>
       <c r="O5" s="38"/>
     </row>
-    <row r="6" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A6" s="48" t="s">
-        <v>95</v>
+    <row r="6" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A6" s="44" t="s">
+        <v>39</v>
       </c>
       <c r="B6" s="37">
-        <v>780</v>
+        <v>810</v>
       </c>
       <c r="C6" s="38">
-        <v>840</v>
+        <v>880</v>
       </c>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
       <c r="H6" s="38"/>
-      <c r="I6" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" s="40">
-        <v>5750</v>
+      <c r="I6" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="39">
+        <v>6540</v>
       </c>
       <c r="K6" s="38">
-        <v>6190</v>
+        <v>6990</v>
       </c>
       <c r="L6" s="38"/>
       <c r="M6" s="38"/>
       <c r="N6" s="38"/>
       <c r="O6" s="38"/>
     </row>
-    <row r="7" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A7" s="48" t="s">
-        <v>97</v>
+    <row r="7" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A7" s="44" t="s">
+        <v>51</v>
       </c>
       <c r="B7" s="37">
-        <v>865</v>
+        <v>800</v>
       </c>
       <c r="C7" s="38">
-        <v>925</v>
+        <v>870</v>
       </c>
       <c r="D7" s="38"/>
       <c r="E7" s="38"/>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
       <c r="H7" s="38"/>
-      <c r="I7" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="J7" s="36">
-        <v>5940</v>
+      <c r="I7" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="39">
+        <v>5290</v>
       </c>
       <c r="K7" s="38">
-        <v>6390</v>
+        <v>5690</v>
       </c>
       <c r="L7" s="38"/>
       <c r="M7" s="38"/>
       <c r="N7" s="38"/>
       <c r="O7" s="38"/>
     </row>
-    <row r="8" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A8" s="48" t="s">
-        <v>39</v>
+    <row r="8" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A8" s="44" t="s">
+        <v>26</v>
       </c>
       <c r="B8" s="37">
-        <v>810</v>
+        <v>790</v>
       </c>
       <c r="C8" s="38">
-        <v>880</v>
+        <v>860</v>
       </c>
       <c r="D8" s="38"/>
       <c r="E8" s="38"/>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
       <c r="H8" s="38"/>
-      <c r="I8" s="48" t="s">
-        <v>49</v>
+      <c r="I8" s="43" t="s">
+        <v>86</v>
       </c>
       <c r="J8" s="39">
-        <v>6530</v>
+        <v>5470</v>
       </c>
       <c r="K8" s="38">
-        <v>6990</v>
+        <v>5890</v>
       </c>
       <c r="L8" s="38"/>
       <c r="M8" s="38"/>
       <c r="N8" s="38"/>
       <c r="O8" s="38"/>
     </row>
-    <row r="9" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A9" s="48" t="s">
-        <v>51</v>
+    <row r="9" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A9" s="44" t="s">
+        <v>94</v>
       </c>
       <c r="B9" s="37">
         <v>800</v>
       </c>
       <c r="C9" s="38">
-        <v>870</v>
+        <v>860</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
-      <c r="I9" s="47" t="s">
-        <v>104</v>
+      <c r="I9" s="44" t="s">
+        <v>68</v>
       </c>
       <c r="J9" s="39">
-        <v>6890</v>
+        <v>5750</v>
       </c>
       <c r="K9" s="38">
-        <v>7490</v>
+        <v>6190</v>
       </c>
       <c r="L9" s="38"/>
       <c r="M9" s="38"/>
       <c r="N9" s="38"/>
       <c r="O9" s="38"/>
     </row>
-    <row r="10" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A10" s="48" t="s">
-        <v>17</v>
+    <row r="10" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A10" s="44" t="s">
+        <v>105</v>
       </c>
       <c r="B10" s="37">
-        <v>795</v>
+        <v>790</v>
       </c>
       <c r="C10" s="38">
-        <v>865</v>
+        <v>850</v>
       </c>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
-      <c r="I10" s="47" t="s">
-        <v>90</v>
+      <c r="I10" s="44" t="s">
+        <v>84</v>
       </c>
       <c r="J10" s="39">
-        <v>8340</v>
+        <v>5940</v>
       </c>
       <c r="K10" s="38">
-        <v>8990</v>
+        <v>6390</v>
       </c>
       <c r="L10" s="38"/>
       <c r="M10" s="38"/>
       <c r="N10" s="38"/>
       <c r="O10" s="38"/>
     </row>
-    <row r="11" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A11" s="48" t="s">
-        <v>26</v>
+    <row r="11" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A11" s="44" t="s">
+        <v>0</v>
       </c>
       <c r="B11" s="37">
-        <v>790</v>
+        <v>915</v>
       </c>
       <c r="C11" s="38">
-        <v>860</v>
+        <v>990</v>
       </c>
       <c r="D11" s="38"/>
       <c r="E11" s="38"/>
       <c r="F11" s="38"/>
       <c r="G11" s="38"/>
       <c r="H11" s="38"/>
-      <c r="I11" s="48" t="s">
-        <v>31</v>
+      <c r="I11" s="43" t="s">
+        <v>49</v>
       </c>
       <c r="J11" s="39">
-        <v>9190</v>
+        <v>6530</v>
       </c>
       <c r="K11" s="38">
-        <v>9990</v>
+        <v>6990</v>
       </c>
       <c r="L11" s="38"/>
       <c r="M11" s="38"/>
       <c r="N11" s="38"/>
       <c r="O11" s="38"/>
     </row>
-    <row r="12" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A12" s="48" t="s">
-        <v>94</v>
+    <row r="12" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A12" s="44" t="s">
+        <v>16</v>
       </c>
       <c r="B12" s="37">
-        <v>800</v>
+        <v>890</v>
       </c>
       <c r="C12" s="38">
-        <v>860</v>
+        <v>970</v>
       </c>
       <c r="D12" s="38"/>
       <c r="E12" s="38"/>
       <c r="F12" s="38"/>
       <c r="G12" s="38"/>
       <c r="H12" s="38"/>
-      <c r="I12" s="47" t="s">
-        <v>71</v>
+      <c r="I12" s="44" t="s">
+        <v>104</v>
       </c>
       <c r="J12" s="39">
-        <v>5750</v>
+        <v>6890</v>
       </c>
       <c r="K12" s="38">
-        <v>6190</v>
+        <v>7490</v>
       </c>
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>
       <c r="N12" s="38"/>
       <c r="O12" s="38"/>
     </row>
-    <row r="13" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A13" s="48" t="s">
-        <v>105</v>
+    <row r="13" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A13" s="44" t="s">
+        <v>2</v>
       </c>
       <c r="B13" s="37">
-        <v>790</v>
+        <v>920</v>
       </c>
       <c r="C13" s="38">
-        <v>850</v>
+        <v>999</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
       <c r="F13" s="38"/>
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
-      <c r="I13" s="48" t="s">
-        <v>76</v>
+      <c r="I13" s="44" t="s">
+        <v>90</v>
       </c>
       <c r="J13" s="39">
-        <v>4280</v>
+        <v>8340</v>
       </c>
       <c r="K13" s="38">
-        <v>4590</v>
+        <v>8990</v>
       </c>
       <c r="L13" s="38"/>
       <c r="M13" s="38"/>
       <c r="N13" s="38"/>
       <c r="O13" s="38"/>
     </row>
-    <row r="14" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A14" s="48" t="s">
-        <v>18</v>
+    <row r="14" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A14" s="44" t="s">
+        <v>35</v>
       </c>
       <c r="B14" s="37">
-        <v>970</v>
+        <v>880</v>
       </c>
       <c r="C14" s="38">
-        <v>1060</v>
+        <v>950</v>
       </c>
       <c r="D14" s="38"/>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
-      <c r="I14" s="47" t="s">
-        <v>14</v>
+      <c r="I14" s="44" t="s">
+        <v>31</v>
       </c>
       <c r="J14" s="39">
-        <v>5650</v>
+        <v>9190</v>
       </c>
       <c r="K14" s="38">
-        <v>6150</v>
+        <v>9990</v>
       </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
       <c r="N14" s="38"/>
       <c r="O14" s="38"/>
     </row>
-    <row r="15" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="48" t="s">
-        <v>73</v>
+    <row r="15" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A15" s="44" t="s">
+        <v>103</v>
       </c>
       <c r="B15" s="37">
-        <v>900</v>
+        <v>845</v>
       </c>
       <c r="C15" s="38">
-        <v>975</v>
+        <v>910</v>
       </c>
       <c r="D15" s="38"/>
       <c r="E15" s="38"/>
       <c r="F15" s="38"/>
       <c r="G15" s="38"/>
       <c r="H15" s="38"/>
-      <c r="I15" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="J15" s="39">
-        <v>5020</v>
-      </c>
-      <c r="K15" s="38">
-        <v>5390</v>
+      <c r="I15" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="40">
+        <v>5750</v>
+      </c>
+      <c r="K15" s="46">
+        <v>6190</v>
       </c>
       <c r="L15" s="38"/>
       <c r="M15" s="38"/>
       <c r="N15" s="38"/>
       <c r="O15" s="38"/>
     </row>
-    <row r="16" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A16" s="48" t="s">
-        <v>0</v>
+    <row r="16" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A16" s="44" t="s">
+        <v>18</v>
       </c>
       <c r="B16" s="37">
-        <v>915</v>
+        <v>970</v>
       </c>
       <c r="C16" s="38">
-        <v>990</v>
+        <v>1060</v>
       </c>
       <c r="D16" s="38"/>
       <c r="E16" s="38"/>
       <c r="F16" s="38"/>
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
-      <c r="I16" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="39">
-        <v>5280</v>
-      </c>
-      <c r="K16" s="38">
-        <v>5690</v>
+      <c r="I16" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="40">
+        <v>3560</v>
+      </c>
+      <c r="K16" s="46">
+        <v>3840</v>
       </c>
       <c r="L16" s="38"/>
       <c r="M16" s="38"/>
       <c r="N16" s="38"/>
       <c r="O16" s="38"/>
     </row>
-    <row r="17" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A17" s="48" t="s">
-        <v>52</v>
+    <row r="17" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A17" s="44" t="s">
+        <v>3</v>
       </c>
       <c r="B17" s="37">
-        <v>910</v>
+        <v>1000</v>
       </c>
       <c r="C17" s="38">
-        <v>980</v>
+        <v>1090</v>
       </c>
       <c r="D17" s="38"/>
       <c r="E17" s="38"/>
       <c r="F17" s="38"/>
       <c r="G17" s="38"/>
       <c r="H17" s="38"/>
-      <c r="I17" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="J17" s="39">
-        <v>4550</v>
-      </c>
-      <c r="K17" s="38">
-        <v>4890</v>
+      <c r="I17" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="J17" s="40">
+        <v>3340</v>
+      </c>
+      <c r="K17" s="46">
+        <v>3590</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="38"/>
       <c r="N17" s="38"/>
       <c r="O17" s="38"/>
     </row>
-    <row r="18" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A18" s="48" t="s">
-        <v>16</v>
+    <row r="18" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A18" s="44" t="s">
+        <v>1</v>
       </c>
       <c r="B18" s="37">
-        <v>890</v>
+        <v>995</v>
       </c>
       <c r="C18" s="38">
-        <v>970</v>
+        <v>1075</v>
       </c>
       <c r="D18" s="38"/>
       <c r="E18" s="38"/>
       <c r="F18" s="38"/>
       <c r="G18" s="38"/>
       <c r="H18" s="38"/>
-      <c r="I18" s="47" t="s">
-        <v>50</v>
+      <c r="I18" s="44" t="s">
+        <v>91</v>
       </c>
       <c r="J18" s="39">
-        <v>5100</v>
-      </c>
-      <c r="K18" s="38">
-        <v>5490</v>
+        <v>4500</v>
+      </c>
+      <c r="K18" s="46">
+        <v>4790</v>
       </c>
       <c r="L18" s="38"/>
       <c r="M18" s="38"/>
       <c r="N18" s="38"/>
       <c r="O18" s="38"/>
     </row>
-    <row r="19" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A19" s="48" t="s">
-        <v>2</v>
+    <row r="19" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A19" s="44" t="s">
+        <v>102</v>
       </c>
       <c r="B19" s="37">
-        <v>920</v>
+        <v>880</v>
       </c>
       <c r="C19" s="38">
-        <v>999</v>
+        <v>950</v>
       </c>
       <c r="D19" s="38"/>
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
       <c r="G19" s="38"/>
       <c r="H19" s="38"/>
-      <c r="I19" s="48" t="s">
-        <v>33</v>
+      <c r="I19" s="43" t="s">
+        <v>21</v>
       </c>
       <c r="J19" s="39">
-        <v>5560</v>
-      </c>
-      <c r="K19" s="38">
-        <v>5990</v>
+        <v>3710</v>
+      </c>
+      <c r="K19" s="46">
+        <v>3990</v>
       </c>
       <c r="L19" s="38"/>
       <c r="M19" s="38"/>
       <c r="N19" s="38"/>
       <c r="O19" s="38"/>
     </row>
-    <row r="20" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A20" s="48" t="s">
-        <v>35</v>
+    <row r="20" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A20" s="44" t="s">
+        <v>43</v>
       </c>
       <c r="B20" s="37">
-        <v>880</v>
+        <v>900</v>
       </c>
       <c r="C20" s="38">
-        <v>950</v>
+        <v>970</v>
       </c>
       <c r="D20" s="38"/>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
       <c r="G20" s="38"/>
       <c r="H20" s="38"/>
-      <c r="I20" s="48" t="s">
-        <v>45</v>
+      <c r="I20" s="43" t="s">
+        <v>92</v>
       </c>
       <c r="J20" s="39">
-        <v>6090</v>
+        <v>3620</v>
       </c>
       <c r="K20" s="38">
-        <v>6590</v>
+        <v>3890</v>
       </c>
       <c r="L20" s="38"/>
       <c r="M20" s="38"/>
       <c r="N20" s="38"/>
       <c r="O20" s="38"/>
     </row>
-    <row r="21" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A21" s="48" t="s">
-        <v>103</v>
+    <row r="21" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A21" s="44" t="s">
+        <v>41</v>
       </c>
       <c r="B21" s="37">
-        <v>845</v>
+        <v>1040</v>
       </c>
       <c r="C21" s="38">
-        <v>910</v>
+        <v>1120</v>
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
       <c r="H21" s="38"/>
-      <c r="I21" s="48" t="s">
-        <v>36</v>
+      <c r="I21" s="43" t="s">
+        <v>54</v>
       </c>
       <c r="J21" s="39">
-        <v>5390</v>
+        <v>4080</v>
       </c>
       <c r="K21" s="38">
-        <v>5790</v>
+        <v>4390</v>
       </c>
       <c r="L21" s="38"/>
       <c r="M21" s="38"/>
       <c r="N21" s="38"/>
       <c r="O21" s="38"/>
     </row>
-    <row r="22" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A22" s="48" t="s">
-        <v>3</v>
+    <row r="22" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A22" s="44" t="s">
+        <v>98</v>
       </c>
       <c r="B22" s="37">
-        <v>1000</v>
+        <v>930</v>
       </c>
       <c r="C22" s="38">
-        <v>1090</v>
+        <v>999</v>
       </c>
       <c r="D22" s="38"/>
       <c r="E22" s="38"/>
       <c r="F22" s="38"/>
       <c r="G22" s="38"/>
       <c r="H22" s="38"/>
-      <c r="I22" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="J22" s="39">
-        <v>3630</v>
+      <c r="I22" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="J22" s="40">
+        <v>4220</v>
       </c>
       <c r="K22" s="38">
-        <v>3890</v>
+        <v>4540</v>
       </c>
       <c r="L22" s="38"/>
       <c r="M22" s="38"/>
       <c r="N22" s="38"/>
       <c r="O22" s="38"/>
     </row>
-    <row r="23" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A23" s="48" t="s">
-        <v>1</v>
+    <row r="23" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A23" s="44" t="s">
+        <v>70</v>
       </c>
       <c r="B23" s="37">
-        <v>995</v>
+        <v>1190</v>
       </c>
       <c r="C23" s="38">
-        <v>1075</v>
+        <v>1290</v>
       </c>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
       <c r="F23" s="38"/>
       <c r="G23" s="38"/>
       <c r="H23" s="38"/>
-      <c r="I23" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="J23" s="39">
-        <v>3560</v>
+      <c r="I23" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="J23" s="40">
+        <v>3710</v>
       </c>
       <c r="K23" s="38">
-        <v>3840</v>
+        <v>3990</v>
       </c>
       <c r="L23" s="38"/>
       <c r="M23" s="38"/>
       <c r="N23" s="38"/>
       <c r="O23" s="38"/>
     </row>
-    <row r="24" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A24" s="48" t="s">
-        <v>102</v>
+    <row r="24" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A24" s="44" t="s">
+        <v>72</v>
       </c>
       <c r="B24" s="37">
-        <v>880</v>
+        <v>1170</v>
       </c>
       <c r="C24" s="38">
-        <v>950</v>
+        <v>1270</v>
       </c>
       <c r="D24" s="38"/>
       <c r="E24" s="38"/>
       <c r="F24" s="38"/>
       <c r="G24" s="38"/>
       <c r="H24" s="38"/>
-      <c r="I24" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="J24" s="39">
-        <v>3340</v>
+      <c r="I24" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="J24" s="40">
+        <v>4280</v>
       </c>
       <c r="K24" s="38">
-        <v>3590</v>
+        <v>4590</v>
       </c>
       <c r="L24" s="38"/>
       <c r="M24" s="38"/>
       <c r="N24" s="38"/>
       <c r="O24" s="38"/>
     </row>
-    <row r="25" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A25" s="48" t="s">
-        <v>43</v>
+    <row r="25" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A25" s="44" t="s">
+        <v>19</v>
       </c>
       <c r="B25" s="37">
-        <v>900</v>
+        <v>1190</v>
       </c>
       <c r="C25" s="38">
-        <v>970</v>
+        <v>1290</v>
       </c>
       <c r="D25" s="38"/>
       <c r="E25" s="38"/>
       <c r="F25" s="38"/>
       <c r="G25" s="38"/>
       <c r="H25" s="38"/>
-      <c r="I25" s="48" t="s">
-        <v>53</v>
+      <c r="I25" s="43" t="s">
+        <v>28</v>
       </c>
       <c r="J25" s="39">
+        <v>5020</v>
+      </c>
+      <c r="K25" s="38">
         <v>5390</v>
-      </c>
-      <c r="K25" s="38">
-        <v>5790</v>
       </c>
       <c r="L25" s="38"/>
       <c r="M25" s="38"/>
       <c r="N25" s="38"/>
       <c r="O25" s="38"/>
-    </row>
-    <row r="26" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A26" s="48" t="s">
-        <v>41</v>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="35"/>
+      <c r="U25" s="35"/>
+    </row>
+    <row r="26" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A26" s="44" t="s">
+        <v>15</v>
       </c>
       <c r="B26" s="37">
-        <v>1040</v>
-      </c>
-      <c r="C26" s="38">
-        <v>1120</v>
+        <v>1080</v>
+      </c>
+      <c r="C26" s="46">
+        <v>1160</v>
       </c>
       <c r="D26" s="38"/>
       <c r="E26" s="38"/>
       <c r="F26" s="38"/>
       <c r="G26" s="38"/>
       <c r="H26" s="38"/>
-      <c r="I26" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="J26" s="39">
-        <v>4500</v>
+      <c r="I26" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="40">
+        <v>5280</v>
       </c>
       <c r="K26" s="38">
-        <v>4790</v>
+        <v>5690</v>
       </c>
       <c r="L26" s="38"/>
       <c r="M26" s="38"/>
       <c r="N26" s="38"/>
       <c r="O26" s="38"/>
-    </row>
-    <row r="27" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A27" s="48" t="s">
-        <v>98</v>
+      <c r="R26" s="94"/>
+      <c r="S26" s="95"/>
+      <c r="T26" s="96"/>
+      <c r="U26" s="35"/>
+    </row>
+    <row r="27" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A27" s="44" t="s">
+        <v>30</v>
       </c>
       <c r="B27" s="37">
-        <v>930</v>
-      </c>
-      <c r="C27" s="38">
-        <v>999</v>
+        <v>1100</v>
+      </c>
+      <c r="C27" s="46">
+        <v>1199</v>
       </c>
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
       <c r="F27" s="38"/>
       <c r="G27" s="38"/>
       <c r="H27" s="38"/>
-      <c r="I27" s="47" t="s">
-        <v>46</v>
+      <c r="I27" s="44" t="s">
+        <v>99</v>
       </c>
       <c r="J27" s="39">
-        <v>4970</v>
+        <v>4550</v>
       </c>
       <c r="K27" s="38">
-        <v>5290</v>
+        <v>4890</v>
       </c>
       <c r="L27" s="38"/>
       <c r="M27" s="38"/>
       <c r="N27" s="38"/>
       <c r="O27" s="38"/>
-    </row>
-    <row r="28" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A28" s="48" t="s">
-        <v>74</v>
+      <c r="R27" s="94"/>
+      <c r="S27" s="95"/>
+      <c r="T27" s="96"/>
+      <c r="U27" s="35"/>
+    </row>
+    <row r="28" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A28" s="44" t="s">
+        <v>24</v>
       </c>
       <c r="B28" s="37">
-        <v>1290</v>
-      </c>
-      <c r="C28" s="38">
-        <v>1390</v>
+        <v>1010</v>
+      </c>
+      <c r="C28" s="46">
+        <v>1110</v>
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
       <c r="F28" s="38"/>
       <c r="G28" s="38"/>
       <c r="H28" s="38"/>
-      <c r="I28" s="47" t="s">
-        <v>79</v>
+      <c r="I28" s="43" t="s">
+        <v>50</v>
       </c>
       <c r="J28" s="39">
-        <v>4015</v>
+        <v>5100</v>
       </c>
       <c r="K28" s="38">
-        <v>4390</v>
+        <v>5490</v>
       </c>
       <c r="L28" s="38"/>
       <c r="M28" s="38"/>
       <c r="N28" s="38"/>
       <c r="O28" s="38"/>
-    </row>
-    <row r="29" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A29" s="48" t="s">
-        <v>70</v>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
+    </row>
+    <row r="29" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A29" s="44" t="s">
+        <v>34</v>
       </c>
       <c r="B29" s="37">
-        <v>1190</v>
-      </c>
-      <c r="C29" s="38">
-        <v>1290</v>
+        <v>1040</v>
+      </c>
+      <c r="C29" s="46">
+        <v>1130</v>
       </c>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
       <c r="F29" s="38"/>
       <c r="G29" s="38"/>
       <c r="H29" s="38"/>
-      <c r="I29" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="J29" s="40">
-        <v>3710</v>
+      <c r="I29" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="J29" s="39">
+        <v>5390</v>
       </c>
       <c r="K29" s="38">
-        <v>3990</v>
+        <v>5790</v>
       </c>
       <c r="L29" s="38"/>
       <c r="M29" s="38"/>
       <c r="N29" s="38"/>
       <c r="O29" s="38"/>
     </row>
-    <row r="30" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A30" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="37">
-        <v>1270</v>
-      </c>
-      <c r="C30" s="38">
-        <v>1370</v>
-      </c>
+    <row r="30" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A30" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="46"/>
       <c r="D30" s="38"/>
       <c r="E30" s="38"/>
       <c r="F30" s="38"/>
       <c r="G30" s="38"/>
       <c r="H30" s="38"/>
-      <c r="I30" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="J30" s="40">
-        <v>3620</v>
+      <c r="I30" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="39">
+        <v>12090</v>
       </c>
       <c r="K30" s="38">
-        <v>3890</v>
+        <v>12990</v>
       </c>
       <c r="L30" s="38"/>
       <c r="M30" s="38"/>
       <c r="N30" s="38"/>
       <c r="O30" s="38"/>
     </row>
-    <row r="31" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A31" s="48" t="s">
-        <v>72</v>
+    <row r="31" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A31" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="B31" s="37">
-        <v>1170</v>
-      </c>
-      <c r="C31" s="38">
-        <v>1270</v>
+        <v>1100</v>
+      </c>
+      <c r="C31" s="46">
+        <v>1199</v>
       </c>
       <c r="D31" s="38"/>
       <c r="E31" s="38"/>
       <c r="F31" s="38"/>
       <c r="G31" s="38"/>
       <c r="H31" s="38"/>
-      <c r="I31" s="47" t="s">
-        <v>13</v>
-      </c>
-      <c r="J31" s="40">
-        <v>4620</v>
+      <c r="I31" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="J31" s="39">
+        <v>12240</v>
       </c>
       <c r="K31" s="38">
-        <v>4999</v>
+        <v>12990</v>
       </c>
       <c r="L31" s="38"/>
       <c r="M31" s="38"/>
       <c r="N31" s="38"/>
       <c r="O31" s="38"/>
     </row>
-    <row r="32" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A32" s="48" t="s">
-        <v>19</v>
+    <row r="32" spans="1:21" ht="19.5" customHeight="1">
+      <c r="A32" s="44" t="s">
+        <v>66</v>
       </c>
       <c r="B32" s="37">
-        <v>1190</v>
-      </c>
-      <c r="C32" s="38">
-        <v>1290</v>
+        <v>1050</v>
+      </c>
+      <c r="C32" s="46">
+        <v>1130</v>
       </c>
       <c r="D32" s="38"/>
       <c r="E32" s="38"/>
       <c r="F32" s="38"/>
       <c r="G32" s="38"/>
       <c r="H32" s="38"/>
-      <c r="I32" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="J32" s="39">
-        <v>4520</v>
+      <c r="I32" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="J32" s="40">
+        <v>8820</v>
       </c>
       <c r="K32" s="38">
-        <v>4899</v>
+        <v>9490</v>
       </c>
       <c r="L32" s="38"/>
       <c r="M32" s="38"/>
       <c r="N32" s="38"/>
       <c r="O32" s="38"/>
     </row>
-    <row r="33" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A33" s="48" t="s">
-        <v>75</v>
+    <row r="33" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A33" s="44" t="s">
+        <v>40</v>
       </c>
       <c r="B33" s="37">
-        <v>1225</v>
-      </c>
-      <c r="C33" s="38">
-        <v>1325</v>
+        <v>1130</v>
+      </c>
+      <c r="C33" s="46">
+        <v>1230</v>
       </c>
       <c r="D33" s="38"/>
       <c r="E33" s="38"/>
       <c r="F33" s="38"/>
       <c r="G33" s="38"/>
       <c r="H33" s="38"/>
-      <c r="I33" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="J33" s="40">
-        <v>4080</v>
-      </c>
-      <c r="K33" s="38">
-        <v>4390</v>
-      </c>
+      <c r="I33" s="43"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="38"/>
       <c r="L33" s="38"/>
       <c r="M33" s="38"/>
       <c r="N33" s="38"/>
       <c r="O33" s="38"/>
     </row>
-    <row r="34" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A34" s="48" t="s">
-        <v>27</v>
+    <row r="34" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A34" s="44" t="s">
+        <v>32</v>
       </c>
       <c r="B34" s="37">
-        <v>1220</v>
-      </c>
-      <c r="C34" s="38">
-        <v>1320</v>
+        <v>1100</v>
+      </c>
+      <c r="C34" s="46">
+        <v>1190</v>
       </c>
       <c r="D34" s="38"/>
       <c r="E34" s="38"/>
       <c r="F34" s="38"/>
       <c r="G34" s="38"/>
       <c r="H34" s="38"/>
-      <c r="I34" s="48" t="s">
-        <v>93</v>
-      </c>
-      <c r="J34" s="39">
-        <v>4220</v>
-      </c>
-      <c r="K34" s="38">
-        <v>4540</v>
-      </c>
+      <c r="I34" s="43"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="38"/>
       <c r="L34" s="38"/>
       <c r="M34" s="38"/>
       <c r="N34" s="38"/>
       <c r="O34" s="38"/>
     </row>
-    <row r="35" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A35" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="41">
-        <v>1080</v>
-      </c>
-      <c r="C35" s="38">
-        <v>1160</v>
+    <row r="35" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A35" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="37">
+        <v>1330</v>
+      </c>
+      <c r="C35" s="46">
+        <v>1450</v>
       </c>
       <c r="D35" s="38"/>
       <c r="E35" s="38"/>
       <c r="F35" s="38"/>
       <c r="G35" s="38"/>
       <c r="H35" s="38"/>
-      <c r="I35" s="47" t="s">
-        <v>118</v>
-      </c>
+      <c r="I35" s="43"/>
       <c r="J35" s="39"/>
       <c r="K35" s="38"/>
       <c r="L35" s="38"/>
@@ -4929,639 +4927,422 @@
       <c r="N35" s="38"/>
       <c r="O35" s="38"/>
     </row>
-    <row r="36" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A36" s="48" t="s">
-        <v>30</v>
+    <row r="36" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A36" s="44" t="s">
+        <v>23</v>
       </c>
       <c r="B36" s="37">
-        <v>1100</v>
-      </c>
-      <c r="C36" s="38">
-        <v>1199</v>
+        <v>1200</v>
+      </c>
+      <c r="C36" s="46">
+        <v>1299</v>
       </c>
       <c r="D36" s="38"/>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
       <c r="H36" s="38"/>
-      <c r="I36" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="J36" s="39">
-        <v>12240</v>
-      </c>
-      <c r="K36" s="38">
-        <v>12990</v>
-      </c>
+      <c r="I36" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" s="72"/>
+      <c r="K36" s="38"/>
       <c r="L36" s="38"/>
-      <c r="M36" s="38"/>
-      <c r="N36" s="38"/>
-      <c r="O36" s="38"/>
-    </row>
-    <row r="37" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A37" s="48" t="s">
-        <v>67</v>
+      <c r="M36" s="72"/>
+      <c r="N36" s="72"/>
+      <c r="O36" s="41"/>
+    </row>
+    <row r="37" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A37" s="44" t="s">
+        <v>27</v>
       </c>
       <c r="B37" s="37">
-        <v>1200</v>
-      </c>
-      <c r="C37" s="38">
-        <v>1290</v>
+        <v>1220</v>
+      </c>
+      <c r="C37" s="46">
+        <v>1320</v>
       </c>
       <c r="D37" s="38"/>
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
       <c r="H37" s="38"/>
-      <c r="I37" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="J37" s="39">
-        <v>12090</v>
-      </c>
-      <c r="K37" s="38">
-        <v>12990</v>
-      </c>
-      <c r="L37" s="38"/>
-      <c r="M37" s="38"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="38"/>
-    </row>
-    <row r="38" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A38" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="37">
-        <v>1010</v>
-      </c>
-      <c r="C38" s="38">
-        <v>1110</v>
+      <c r="I37" s="72"/>
+      <c r="J37" s="72"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="72"/>
+      <c r="M37" s="72"/>
+      <c r="N37" s="72"/>
+      <c r="O37" s="72"/>
+    </row>
+    <row r="38" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A38" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="46">
+        <v>1070</v>
+      </c>
+      <c r="C38" s="46">
+        <v>1160</v>
       </c>
       <c r="D38" s="38"/>
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
       <c r="H38" s="38"/>
-      <c r="I38" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="J38" s="39">
-        <v>10840</v>
-      </c>
-      <c r="K38" s="38">
-        <v>11990</v>
-      </c>
-      <c r="L38" s="38"/>
-      <c r="M38" s="38"/>
-      <c r="N38" s="38"/>
-      <c r="O38" s="38"/>
-    </row>
-    <row r="39" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A39" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="37">
-        <v>1040</v>
-      </c>
-      <c r="C39" s="38">
-        <v>1130</v>
+      <c r="I38" s="100" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="100"/>
+      <c r="K38" s="100"/>
+      <c r="L38" s="100"/>
+      <c r="M38" s="100"/>
+      <c r="N38" s="100"/>
+      <c r="O38" s="74"/>
+    </row>
+    <row r="39" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A39" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" s="46">
+        <v>1200</v>
+      </c>
+      <c r="C39" s="46">
+        <v>1290</v>
       </c>
       <c r="D39" s="38"/>
       <c r="E39" s="38"/>
       <c r="F39" s="38"/>
       <c r="G39" s="38"/>
       <c r="H39" s="38"/>
-      <c r="I39" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="J39" s="40">
-        <v>12490</v>
-      </c>
-      <c r="K39" s="38">
-        <v>13490</v>
-      </c>
-      <c r="L39" s="38"/>
-      <c r="M39" s="38"/>
-      <c r="N39" s="38"/>
-      <c r="O39" s="38"/>
-    </row>
-    <row r="40" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A40" s="48" t="s">
-        <v>115</v>
-      </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="38"/>
+      <c r="I39" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="J39" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="L39" s="72"/>
+      <c r="M39" s="72"/>
+      <c r="N39" s="72"/>
+      <c r="O39" s="75"/>
+    </row>
+    <row r="40" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A40" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
       <c r="D40" s="38"/>
       <c r="E40" s="38"/>
       <c r="F40" s="38"/>
       <c r="G40" s="38"/>
       <c r="H40" s="38"/>
-      <c r="I40" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="J40" s="39">
-        <v>8820</v>
-      </c>
-      <c r="K40" s="38">
-        <v>9490</v>
-      </c>
+      <c r="I40" s="38">
+        <v>1000</v>
+      </c>
+      <c r="J40" s="40"/>
+      <c r="K40" s="38"/>
       <c r="L40" s="38"/>
       <c r="M40" s="38"/>
       <c r="N40" s="38"/>
-      <c r="O40" s="38"/>
-    </row>
-    <row r="41" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A41" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="37">
+      <c r="O40" s="75"/>
+    </row>
+    <row r="41" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A41" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="46">
         <v>1100</v>
       </c>
-      <c r="C41" s="38">
-        <v>1199</v>
+      <c r="C41" s="46">
+        <v>1190</v>
       </c>
       <c r="D41" s="38"/>
       <c r="E41" s="38"/>
       <c r="F41" s="38"/>
       <c r="G41" s="38"/>
       <c r="H41" s="38"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="39"/>
+      <c r="I41" s="38">
+        <v>500</v>
+      </c>
+      <c r="J41" s="40"/>
       <c r="K41" s="38"/>
       <c r="L41" s="38"/>
       <c r="M41" s="38"/>
       <c r="N41" s="38"/>
-      <c r="O41" s="38"/>
-    </row>
-    <row r="42" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A42" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="37">
-        <v>1100</v>
-      </c>
-      <c r="C42" s="38">
-        <v>1199</v>
+      <c r="O41" s="75"/>
+    </row>
+    <row r="42" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A42" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="46">
+        <v>1250</v>
+      </c>
+      <c r="C42" s="46">
+        <v>1350</v>
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="38"/>
       <c r="F42" s="38"/>
       <c r="G42" s="38"/>
       <c r="H42" s="38"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="38">
+        <v>100</v>
+      </c>
+      <c r="J42" s="40"/>
       <c r="K42" s="38"/>
       <c r="L42" s="38"/>
       <c r="M42" s="38"/>
       <c r="N42" s="38"/>
-      <c r="O42" s="38"/>
-    </row>
-    <row r="43" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A43" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="B43" s="37">
-        <v>1050</v>
-      </c>
-      <c r="C43" s="38">
-        <v>1130</v>
+      <c r="O42" s="75"/>
+    </row>
+    <row r="43" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A43" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="46">
+        <v>1370</v>
+      </c>
+      <c r="C43" s="46">
+        <v>1490</v>
       </c>
       <c r="D43" s="38"/>
       <c r="E43" s="38"/>
       <c r="F43" s="38"/>
       <c r="G43" s="38"/>
       <c r="H43" s="38"/>
-      <c r="I43" s="50" t="s">
-        <v>12</v>
-      </c>
-      <c r="J43" s="50"/>
+      <c r="I43" s="38">
+        <v>50</v>
+      </c>
+      <c r="J43" s="40"/>
       <c r="K43" s="38"/>
       <c r="L43" s="38"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="50"/>
-      <c r="O43" s="42"/>
-    </row>
-    <row r="44" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A44" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="B44" s="37">
-        <v>1130</v>
-      </c>
-      <c r="C44" s="38">
-        <v>1230</v>
-      </c>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="75"/>
+    </row>
+    <row r="44" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A44" s="44"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
       <c r="D44" s="38"/>
       <c r="E44" s="38"/>
       <c r="F44" s="38"/>
       <c r="G44" s="38"/>
       <c r="H44" s="38"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="50"/>
-      <c r="K44" s="50"/>
-      <c r="L44" s="50"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="50"/>
-    </row>
-    <row r="45" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A45" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" s="37">
-        <v>1100</v>
-      </c>
-      <c r="C45" s="38">
-        <v>1190</v>
-      </c>
+      <c r="I44" s="38">
+        <v>20</v>
+      </c>
+      <c r="J44" s="40"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="75"/>
+    </row>
+    <row r="45" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A45" s="45"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
       <c r="D45" s="38"/>
       <c r="E45" s="38"/>
       <c r="F45" s="38"/>
       <c r="G45" s="38"/>
       <c r="H45" s="38"/>
-      <c r="I45" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="J45" s="52"/>
-      <c r="K45" s="52"/>
-      <c r="L45" s="52"/>
-      <c r="M45" s="52"/>
-      <c r="N45" s="52"/>
-      <c r="O45" s="53"/>
-    </row>
-    <row r="46" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A46" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="37">
-        <v>1330</v>
-      </c>
-      <c r="C46" s="38">
-        <v>1450</v>
-      </c>
+      <c r="I45" s="38">
+        <v>10</v>
+      </c>
+      <c r="J45" s="40"/>
+      <c r="K45" s="38"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="38"/>
+      <c r="N45" s="38"/>
+      <c r="O45" s="75"/>
+    </row>
+    <row r="46" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A46" s="45"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="38"/>
       <c r="D46" s="38"/>
       <c r="E46" s="38"/>
       <c r="F46" s="38"/>
       <c r="G46" s="38"/>
       <c r="H46" s="38"/>
-      <c r="I46" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="J46" s="40" t="s">
-        <v>9</v>
-      </c>
-      <c r="K46" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="L46" s="50"/>
-      <c r="M46" s="50"/>
-      <c r="N46" s="50"/>
-      <c r="O46" s="54"/>
-    </row>
-    <row r="47" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A47" s="48" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="37">
-        <v>1200</v>
-      </c>
-      <c r="C47" s="38">
-        <v>1299</v>
-      </c>
+      <c r="I46" s="38">
+        <v>5</v>
+      </c>
+      <c r="J46" s="40"/>
+      <c r="K46" s="38"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="38"/>
+      <c r="N46" s="38"/>
+      <c r="O46" s="75"/>
+    </row>
+    <row r="47" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A47" s="45"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
       <c r="D47" s="38"/>
       <c r="E47" s="38"/>
       <c r="F47" s="38"/>
       <c r="G47" s="38"/>
       <c r="H47" s="38"/>
       <c r="I47" s="38">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="J47" s="40"/>
       <c r="K47" s="38"/>
       <c r="L47" s="38"/>
       <c r="M47" s="38"/>
       <c r="N47" s="38"/>
-      <c r="O47" s="54"/>
-    </row>
-    <row r="48" spans="1:15" ht="17.100000000000001" customHeight="1">
-      <c r="A48" s="48" t="s">
-        <v>116</v>
-      </c>
-      <c r="B48" s="37">
-        <v>1070</v>
-      </c>
-      <c r="C48" s="38">
-        <v>1160</v>
-      </c>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38">
-        <v>500</v>
-      </c>
-      <c r="J48" s="40"/>
+      <c r="O47" s="75"/>
+    </row>
+    <row r="48" spans="1:15" ht="19.5" customHeight="1">
+      <c r="A48" s="44"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="J48" s="38"/>
       <c r="K48" s="38"/>
       <c r="L48" s="38"/>
       <c r="M48" s="38"/>
       <c r="N48" s="38"/>
-      <c r="O48" s="54"/>
-    </row>
-    <row r="49" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A49" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="B49" s="38">
-        <v>1250</v>
-      </c>
-      <c r="C49" s="38">
-        <v>1350</v>
-      </c>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38">
-        <v>100</v>
-      </c>
-      <c r="J49" s="40"/>
-      <c r="K49" s="38"/>
-      <c r="L49" s="38"/>
-      <c r="M49" s="38"/>
-      <c r="N49" s="38"/>
+      <c r="O48" s="76"/>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
+      <c r="I49" s="51"/>
+      <c r="J49" s="51"/>
+      <c r="K49" s="51"/>
+      <c r="L49" s="32"/>
+      <c r="M49" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="N49" s="53"/>
       <c r="O49" s="54"/>
     </row>
-    <row r="50" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A50" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="B50" s="38">
-        <v>1370</v>
-      </c>
-      <c r="C50" s="38">
-        <v>1490</v>
-      </c>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="38">
-        <v>50</v>
-      </c>
-      <c r="J50" s="40"/>
-      <c r="K50" s="38"/>
-      <c r="L50" s="38"/>
-      <c r="M50" s="38"/>
-      <c r="N50" s="38"/>
-      <c r="O50" s="54"/>
-    </row>
-    <row r="51" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A51" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="38">
-        <v>20</v>
-      </c>
-      <c r="J51" s="40"/>
-      <c r="K51" s="38"/>
-      <c r="L51" s="38"/>
-      <c r="M51" s="38"/>
-      <c r="N51" s="38"/>
-      <c r="O51" s="54"/>
-    </row>
-    <row r="52" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A52" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="B52" s="38">
-        <v>1100</v>
-      </c>
-      <c r="C52" s="38">
-        <v>1190</v>
-      </c>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="38">
-        <v>10</v>
-      </c>
-      <c r="J52" s="40"/>
-      <c r="K52" s="38"/>
-      <c r="L52" s="38"/>
-      <c r="M52" s="38"/>
-      <c r="N52" s="38"/>
-      <c r="O52" s="54"/>
-    </row>
-    <row r="53" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A53" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="38">
-        <v>2780</v>
-      </c>
-      <c r="C53" s="38">
-        <v>2990</v>
-      </c>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38">
-        <v>5</v>
-      </c>
-      <c r="J53" s="40"/>
-      <c r="K53" s="38"/>
-      <c r="L53" s="38"/>
-      <c r="M53" s="38"/>
-      <c r="N53" s="38"/>
-      <c r="O53" s="54"/>
-    </row>
-    <row r="54" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A54" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="B54" s="38">
-        <v>6540</v>
-      </c>
-      <c r="C54" s="38">
-        <v>6990</v>
-      </c>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="38">
-        <v>2</v>
-      </c>
-      <c r="J54" s="40"/>
-      <c r="K54" s="38"/>
-      <c r="L54" s="38"/>
-      <c r="M54" s="38"/>
-      <c r="N54" s="38"/>
-      <c r="O54" s="54"/>
-    </row>
-    <row r="55" spans="1:16" ht="17.100000000000001" customHeight="1">
-      <c r="A55" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="B55" s="36">
-        <v>5290</v>
-      </c>
-      <c r="C55" s="36">
-        <v>5690</v>
-      </c>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="J55" s="38"/>
-      <c r="K55" s="38"/>
-      <c r="L55" s="38"/>
-      <c r="M55" s="38"/>
-      <c r="N55" s="38"/>
-      <c r="O55" s="55"/>
-    </row>
-    <row r="56" spans="1:16">
-      <c r="A56" s="63" t="s">
-        <v>107</v>
-      </c>
-      <c r="B56" s="64"/>
-      <c r="C56" s="64"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="67" t="s">
-        <v>108</v>
-      </c>
-      <c r="F56" s="67"/>
-      <c r="G56" s="67"/>
-      <c r="H56" s="67"/>
-      <c r="I56" s="67"/>
-      <c r="J56" s="67"/>
-      <c r="K56" s="67"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="69" t="s">
-        <v>106</v>
-      </c>
-      <c r="N56" s="69"/>
-      <c r="O56" s="70"/>
-    </row>
-    <row r="57" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A57" s="65"/>
-      <c r="B57" s="66"/>
-      <c r="C57" s="66"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="68"/>
-      <c r="F57" s="68"/>
-      <c r="G57" s="68"/>
-      <c r="H57" s="68"/>
-      <c r="I57" s="68"/>
-      <c r="J57" s="68"/>
-      <c r="K57" s="68"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="71"/>
-      <c r="N57" s="71"/>
-      <c r="O57" s="72"/>
-    </row>
-    <row r="58" spans="1:16">
-      <c r="A58" s="29"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29"/>
-      <c r="I58" s="29"/>
-      <c r="J58" s="26"/>
-      <c r="K58" s="26"/>
-      <c r="L58" s="26"/>
-      <c r="M58" s="26"/>
-      <c r="N58" s="30"/>
-      <c r="O58" s="30"/>
-    </row>
-    <row r="59" spans="1:16">
-      <c r="A59" s="73" t="s">
+    <row r="50" spans="1:16" ht="15.75" customHeight="1">
+      <c r="A50" s="49"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="52"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="52"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="52"/>
+      <c r="K50" s="52"/>
+      <c r="L50" s="33"/>
+      <c r="M50" s="55"/>
+      <c r="N50" s="55"/>
+      <c r="O50" s="56"/>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="26"/>
+      <c r="K51" s="26"/>
+      <c r="L51" s="26"/>
+      <c r="M51" s="26"/>
+      <c r="N51" s="30"/>
+      <c r="O51" s="30"/>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="B59" s="73"/>
-      <c r="C59" s="73"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29"/>
-      <c r="G59" s="75" t="s">
+      <c r="B52" s="57"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="H59" s="76"/>
-      <c r="I59" s="77"/>
-      <c r="J59" s="29"/>
-      <c r="K59" s="29"/>
-      <c r="L59" s="35"/>
-      <c r="M59" s="74" t="s">
+      <c r="H52" s="60"/>
+      <c r="I52" s="61"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="N59" s="74"/>
-      <c r="O59" s="74"/>
-    </row>
-    <row r="60" spans="1:16">
-      <c r="A60" s="34"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29"/>
-      <c r="G60" s="78"/>
-      <c r="H60" s="79"/>
-      <c r="I60" s="80"/>
-      <c r="J60" s="29"/>
-      <c r="K60" s="29"/>
-      <c r="L60" s="35"/>
-      <c r="M60" s="29"/>
-      <c r="N60" s="29"/>
-      <c r="O60" s="29"/>
-    </row>
-    <row r="64" spans="1:16">
-      <c r="P64" s="35"/>
+      <c r="N52" s="58"/>
+      <c r="O52" s="58"/>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" s="34"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="63"/>
+      <c r="I53" s="64"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="29"/>
+      <c r="L53" s="35"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="29"/>
+      <c r="O53" s="29"/>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="P57" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A56:C57"/>
-    <mergeCell ref="E56:K57"/>
-    <mergeCell ref="M56:O57"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="M59:O59"/>
-    <mergeCell ref="G59:I60"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="I37:O37"/>
+    <mergeCell ref="I38:N38"/>
+    <mergeCell ref="O38:O48"/>
+    <mergeCell ref="K39:N39"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="I44:O44"/>
-    <mergeCell ref="I45:N45"/>
-    <mergeCell ref="O45:O55"/>
-    <mergeCell ref="K46:N46"/>
+    <mergeCell ref="A49:C50"/>
+    <mergeCell ref="E49:K50"/>
+    <mergeCell ref="M49:O50"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="M52:O52"/>
+    <mergeCell ref="G52:I53"/>
   </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
   <pageSetup scale="76" orientation="portrait" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
@@ -5596,73 +5377,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="85" t="s">
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="91" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="83" t="s">
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="92" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="87"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="93"/>
+      <c r="N3" s="93"/>
+      <c r="O3" s="93"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="87" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5670,12 +5451,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="82" t="s">
+      <c r="L4" s="88" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="88"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="6" t="s">
@@ -6779,14 +6560,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="88" t="s">
+      <c r="I44" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="89"/>
+      <c r="J44" s="82"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="88"/>
-      <c r="N44" s="88"/>
+      <c r="M44" s="81"/>
+      <c r="N44" s="81"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -6804,13 +6585,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="88"/>
-      <c r="J45" s="88"/>
-      <c r="K45" s="88"/>
-      <c r="L45" s="88"/>
-      <c r="M45" s="88"/>
-      <c r="N45" s="88"/>
-      <c r="O45" s="88"/>
+      <c r="I45" s="81"/>
+      <c r="J45" s="81"/>
+      <c r="K45" s="81"/>
+      <c r="L45" s="81"/>
+      <c r="M45" s="81"/>
+      <c r="N45" s="81"/>
+      <c r="O45" s="81"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="9" t="s">
@@ -6827,15 +6608,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="90" t="s">
+      <c r="I46" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="90"/>
-      <c r="K46" s="90"/>
-      <c r="L46" s="90"/>
-      <c r="M46" s="90"/>
-      <c r="N46" s="90"/>
-      <c r="O46" s="91"/>
+      <c r="J46" s="83"/>
+      <c r="K46" s="83"/>
+      <c r="L46" s="83"/>
+      <c r="M46" s="83"/>
+      <c r="N46" s="83"/>
+      <c r="O46" s="84"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="9" t="s">
@@ -6858,13 +6639,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="88" t="s">
+      <c r="K47" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="88"/>
-      <c r="M47" s="88"/>
-      <c r="N47" s="88"/>
-      <c r="O47" s="92"/>
+      <c r="L47" s="81"/>
+      <c r="M47" s="81"/>
+      <c r="N47" s="81"/>
+      <c r="O47" s="85"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="9" t="s">
@@ -6889,7 +6670,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="92"/>
+      <c r="O48" s="85"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="9" t="s">
@@ -6914,7 +6695,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="92"/>
+      <c r="O49" s="85"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="4" t="s">
@@ -6939,7 +6720,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="92"/>
+      <c r="O50" s="85"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="4" t="s">
@@ -6964,7 +6745,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="92"/>
+      <c r="O51" s="85"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="4" t="s">
@@ -6989,7 +6770,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="92"/>
+      <c r="O52" s="85"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="4" t="s">
@@ -7014,7 +6795,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="92"/>
+      <c r="O53" s="85"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="4" t="s">
@@ -7039,7 +6820,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="92"/>
+      <c r="O54" s="85"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="4" t="s">
@@ -7064,7 +6845,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="92"/>
+      <c r="O55" s="85"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="9" t="s">
@@ -7089,7 +6870,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="93"/>
+      <c r="O56" s="86"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="17"/>
@@ -7109,49 +6890,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="94" t="s">
+      <c r="A58" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="94"/>
-      <c r="C58" s="94"/>
+      <c r="B58" s="77"/>
+      <c r="C58" s="77"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="97" t="s">
+      <c r="F58" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="97"/>
-      <c r="H58" s="97"/>
-      <c r="I58" s="97"/>
-      <c r="J58" s="97"/>
-      <c r="K58" s="97"/>
+      <c r="G58" s="80"/>
+      <c r="H58" s="80"/>
+      <c r="I58" s="80"/>
+      <c r="J58" s="80"/>
+      <c r="K58" s="80"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="95" t="s">
+      <c r="N58" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="95"/>
+      <c r="O58" s="78"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="96"/>
-      <c r="B59" s="96"/>
-      <c r="C59" s="96"/>
+      <c r="A59" s="79"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="79"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="97"/>
-      <c r="G59" s="97"/>
-      <c r="H59" s="97"/>
-      <c r="I59" s="97"/>
-      <c r="J59" s="97"/>
-      <c r="K59" s="97"/>
+      <c r="F59" s="80"/>
+      <c r="G59" s="80"/>
+      <c r="H59" s="80"/>
+      <c r="I59" s="80"/>
+      <c r="J59" s="80"/>
+      <c r="K59" s="80"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="96"/>
-      <c r="O59" s="96"/>
+      <c r="N59" s="79"/>
+      <c r="O59" s="79"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="96"/>
-      <c r="B60" s="96"/>
-      <c r="C60" s="96"/>
+      <c r="A60" s="79"/>
+      <c r="B60" s="79"/>
+      <c r="C60" s="79"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -7162,15 +6943,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="96"/>
-      <c r="O60" s="96"/>
+      <c r="N60" s="79"/>
+      <c r="O60" s="79"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="94" t="s">
+      <c r="A61" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="94"/>
-      <c r="C61" s="94"/>
+      <c r="B61" s="77"/>
+      <c r="C61" s="77"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -7181,11 +6962,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="95"/>
-      <c r="O61" s="95"/>
+      <c r="N61" s="78"/>
+      <c r="O61" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="A59:C60"/>
@@ -7193,19 +6987,6 @@
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="N61:O61"/>
     <mergeCell ref="F58:K59"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
05.10.19 Today Sales Info
</commit_message>
<xml_diff>
--- a/October/Others/Allocation Sheet.xlsx
+++ b/October/Others/Allocation Sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="122">
   <si>
     <t>BL60</t>
   </si>
@@ -436,7 +436,10 @@
     <t>L65j</t>
   </si>
   <si>
-    <t>Md Robiul Islam</t>
+    <t>D40i</t>
+  </si>
+  <si>
+    <t>Md Shohel Rana</t>
   </si>
 </sst>
 </file>
@@ -919,6 +922,57 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -973,40 +1027,43 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1021,64 +1078,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1481,7 +1484,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2581,7 +2584,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3027,7 +3030,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3098,7 +3101,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3172,7 +3175,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3243,7 +3246,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3905,8 +3908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection sqref="A1:O53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3929,108 +3932,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="65" t="s">
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
       <c r="A3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="69"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="66" t="s">
+      <c r="K3" s="99" t="s">
         <v>110</v>
       </c>
-      <c r="M3" s="67"/>
-      <c r="N3" s="68" t="s">
-        <v>120</v>
-      </c>
-      <c r="O3" s="69"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="100" t="s">
+        <v>121</v>
+      </c>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
     </row>
     <row r="4" spans="1:15" ht="19.5" customHeight="1" thickTop="1">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="98" t="s">
+      <c r="C4" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="98" t="s">
+      <c r="E4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="98" t="s">
+      <c r="F4" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="98" t="s">
+      <c r="G4" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="98"/>
-      <c r="I4" s="97" t="s">
+      <c r="H4" s="51"/>
+      <c r="I4" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="99" t="s">
+      <c r="J4" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="98" t="s">
+      <c r="K4" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="L4" s="98" t="s">
+      <c r="L4" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="M4" s="98" t="s">
+      <c r="M4" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="98" t="s">
+      <c r="N4" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="98" t="s">
+      <c r="O4" s="51" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4529,13 +4532,13 @@
     </row>
     <row r="22" spans="1:21" ht="19.5" customHeight="1">
       <c r="A22" s="44" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="B22" s="37">
-        <v>930</v>
+        <v>1040</v>
       </c>
       <c r="C22" s="38">
-        <v>999</v>
+        <v>1120</v>
       </c>
       <c r="D22" s="38"/>
       <c r="E22" s="38"/>
@@ -4558,13 +4561,13 @@
     </row>
     <row r="23" spans="1:21" ht="19.5" customHeight="1">
       <c r="A23" s="44" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="B23" s="37">
-        <v>1190</v>
+        <v>930</v>
       </c>
       <c r="C23" s="38">
-        <v>1290</v>
+        <v>999</v>
       </c>
       <c r="D23" s="38"/>
       <c r="E23" s="38"/>
@@ -4587,13 +4590,13 @@
     </row>
     <row r="24" spans="1:21" ht="19.5" customHeight="1">
       <c r="A24" s="44" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B24" s="37">
-        <v>1170</v>
+        <v>1190</v>
       </c>
       <c r="C24" s="38">
-        <v>1270</v>
+        <v>1290</v>
       </c>
       <c r="D24" s="38"/>
       <c r="E24" s="38"/>
@@ -4616,13 +4619,13 @@
     </row>
     <row r="25" spans="1:21" ht="19.5" customHeight="1">
       <c r="A25" s="44" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="B25" s="37">
-        <v>1190</v>
+        <v>1170</v>
       </c>
       <c r="C25" s="38">
-        <v>1290</v>
+        <v>1270</v>
       </c>
       <c r="D25" s="38"/>
       <c r="E25" s="38"/>
@@ -4649,13 +4652,13 @@
     </row>
     <row r="26" spans="1:21" ht="19.5" customHeight="1">
       <c r="A26" s="44" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B26" s="37">
-        <v>1080</v>
+        <v>1190</v>
       </c>
       <c r="C26" s="46">
-        <v>1160</v>
+        <v>1290</v>
       </c>
       <c r="D26" s="38"/>
       <c r="E26" s="38"/>
@@ -4675,20 +4678,20 @@
       <c r="M26" s="38"/>
       <c r="N26" s="38"/>
       <c r="O26" s="38"/>
-      <c r="R26" s="94"/>
-      <c r="S26" s="95"/>
-      <c r="T26" s="96"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="48"/>
+      <c r="T26" s="49"/>
       <c r="U26" s="35"/>
     </row>
     <row r="27" spans="1:21" ht="19.5" customHeight="1">
       <c r="A27" s="44" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B27" s="37">
-        <v>1100</v>
+        <v>1080</v>
       </c>
       <c r="C27" s="46">
-        <v>1199</v>
+        <v>1160</v>
       </c>
       <c r="D27" s="38"/>
       <c r="E27" s="38"/>
@@ -4708,20 +4711,20 @@
       <c r="M27" s="38"/>
       <c r="N27" s="38"/>
       <c r="O27" s="38"/>
-      <c r="R27" s="94"/>
-      <c r="S27" s="95"/>
-      <c r="T27" s="96"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="48"/>
+      <c r="T27" s="49"/>
       <c r="U27" s="35"/>
     </row>
     <row r="28" spans="1:21" ht="19.5" customHeight="1">
       <c r="A28" s="44" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B28" s="37">
-        <v>1010</v>
+        <v>1100</v>
       </c>
       <c r="C28" s="46">
-        <v>1110</v>
+        <v>1199</v>
       </c>
       <c r="D28" s="38"/>
       <c r="E28" s="38"/>
@@ -4748,13 +4751,13 @@
     </row>
     <row r="29" spans="1:21" ht="19.5" customHeight="1">
       <c r="A29" s="44" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B29" s="37">
-        <v>1040</v>
+        <v>1010</v>
       </c>
       <c r="C29" s="46">
-        <v>1130</v>
+        <v>1110</v>
       </c>
       <c r="D29" s="38"/>
       <c r="E29" s="38"/>
@@ -4777,10 +4780,14 @@
     </row>
     <row r="30" spans="1:21" ht="19.5" customHeight="1">
       <c r="A30" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="46"/>
+        <v>34</v>
+      </c>
+      <c r="B30" s="37">
+        <v>1040</v>
+      </c>
+      <c r="C30" s="46">
+        <v>1130</v>
+      </c>
       <c r="D30" s="38"/>
       <c r="E30" s="38"/>
       <c r="F30" s="38"/>
@@ -4802,14 +4809,10 @@
     </row>
     <row r="31" spans="1:21" ht="19.5" customHeight="1">
       <c r="A31" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="37">
-        <v>1100</v>
-      </c>
-      <c r="C31" s="46">
-        <v>1199</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="B31" s="37"/>
+      <c r="C31" s="46"/>
       <c r="D31" s="38"/>
       <c r="E31" s="38"/>
       <c r="F31" s="38"/>
@@ -4831,13 +4834,13 @@
     </row>
     <row r="32" spans="1:21" ht="19.5" customHeight="1">
       <c r="A32" s="44" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B32" s="37">
-        <v>1050</v>
+        <v>1100</v>
       </c>
       <c r="C32" s="46">
-        <v>1130</v>
+        <v>1199</v>
       </c>
       <c r="D32" s="38"/>
       <c r="E32" s="38"/>
@@ -4860,13 +4863,13 @@
     </row>
     <row r="33" spans="1:15" ht="19.5" customHeight="1">
       <c r="A33" s="44" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B33" s="37">
+        <v>1050</v>
+      </c>
+      <c r="C33" s="46">
         <v>1130</v>
-      </c>
-      <c r="C33" s="46">
-        <v>1230</v>
       </c>
       <c r="D33" s="38"/>
       <c r="E33" s="38"/>
@@ -4883,13 +4886,13 @@
     </row>
     <row r="34" spans="1:15" ht="19.5" customHeight="1">
       <c r="A34" s="44" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B34" s="37">
-        <v>1100</v>
+        <v>1130</v>
       </c>
       <c r="C34" s="46">
-        <v>1190</v>
+        <v>1230</v>
       </c>
       <c r="D34" s="38"/>
       <c r="E34" s="38"/>
@@ -4906,13 +4909,13 @@
     </row>
     <row r="35" spans="1:15" ht="19.5" customHeight="1">
       <c r="A35" s="44" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="B35" s="37">
-        <v>1330</v>
+        <v>1100</v>
       </c>
       <c r="C35" s="46">
-        <v>1450</v>
+        <v>1190</v>
       </c>
       <c r="D35" s="38"/>
       <c r="E35" s="38"/>
@@ -4929,86 +4932,86 @@
     </row>
     <row r="36" spans="1:15" ht="19.5" customHeight="1">
       <c r="A36" s="44" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
       <c r="B36" s="37">
-        <v>1200</v>
+        <v>1330</v>
       </c>
       <c r="C36" s="46">
-        <v>1299</v>
+        <v>1450</v>
       </c>
       <c r="D36" s="38"/>
       <c r="E36" s="38"/>
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
       <c r="H36" s="38"/>
-      <c r="I36" s="72" t="s">
+      <c r="I36" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="J36" s="72"/>
+      <c r="J36" s="53"/>
       <c r="K36" s="38"/>
       <c r="L36" s="38"/>
-      <c r="M36" s="72"/>
-      <c r="N36" s="72"/>
+      <c r="M36" s="53"/>
+      <c r="N36" s="53"/>
       <c r="O36" s="41"/>
     </row>
     <row r="37" spans="1:15" ht="19.5" customHeight="1">
       <c r="A37" s="44" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B37" s="37">
-        <v>1220</v>
+        <v>1200</v>
       </c>
       <c r="C37" s="46">
-        <v>1320</v>
+        <v>1299</v>
       </c>
       <c r="D37" s="38"/>
       <c r="E37" s="38"/>
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
       <c r="H37" s="38"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="72"/>
-      <c r="K37" s="72"/>
-      <c r="L37" s="72"/>
-      <c r="M37" s="72"/>
-      <c r="N37" s="72"/>
-      <c r="O37" s="72"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="53"/>
+      <c r="O37" s="53"/>
     </row>
     <row r="38" spans="1:15" ht="19.5" customHeight="1">
       <c r="A38" s="45" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
       <c r="B38" s="46">
-        <v>1070</v>
+        <v>1220</v>
       </c>
       <c r="C38" s="46">
-        <v>1160</v>
+        <v>1320</v>
       </c>
       <c r="D38" s="38"/>
       <c r="E38" s="38"/>
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
       <c r="H38" s="38"/>
-      <c r="I38" s="100" t="s">
+      <c r="I38" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="J38" s="100"/>
-      <c r="K38" s="100"/>
-      <c r="L38" s="100"/>
-      <c r="M38" s="100"/>
-      <c r="N38" s="100"/>
-      <c r="O38" s="74"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="55"/>
+      <c r="M38" s="55"/>
+      <c r="N38" s="55"/>
+      <c r="O38" s="56"/>
     </row>
     <row r="39" spans="1:15" ht="19.5" customHeight="1">
       <c r="A39" s="45" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="B39" s="46">
-        <v>1200</v>
+        <v>1070</v>
       </c>
       <c r="C39" s="46">
-        <v>1290</v>
+        <v>1160</v>
       </c>
       <c r="D39" s="38"/>
       <c r="E39" s="38"/>
@@ -5021,20 +5024,24 @@
       <c r="J39" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="K39" s="72" t="s">
+      <c r="K39" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="L39" s="72"/>
-      <c r="M39" s="72"/>
-      <c r="N39" s="72"/>
-      <c r="O39" s="75"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="53"/>
+      <c r="O39" s="57"/>
     </row>
     <row r="40" spans="1:15" ht="19.5" customHeight="1">
       <c r="A40" s="45" t="s">
-        <v>117</v>
-      </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
+        <v>67</v>
+      </c>
+      <c r="B40" s="46">
+        <v>1200</v>
+      </c>
+      <c r="C40" s="46">
+        <v>1290</v>
+      </c>
       <c r="D40" s="38"/>
       <c r="E40" s="38"/>
       <c r="F40" s="38"/>
@@ -5048,18 +5055,14 @@
       <c r="L40" s="38"/>
       <c r="M40" s="38"/>
       <c r="N40" s="38"/>
-      <c r="O40" s="75"/>
+      <c r="O40" s="57"/>
     </row>
     <row r="41" spans="1:15" ht="19.5" customHeight="1">
       <c r="A41" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" s="46">
-        <v>1100</v>
-      </c>
-      <c r="C41" s="46">
-        <v>1190</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
       <c r="D41" s="38"/>
       <c r="E41" s="38"/>
       <c r="F41" s="38"/>
@@ -5073,17 +5076,17 @@
       <c r="L41" s="38"/>
       <c r="M41" s="38"/>
       <c r="N41" s="38"/>
-      <c r="O41" s="75"/>
+      <c r="O41" s="57"/>
     </row>
     <row r="42" spans="1:15" ht="19.5" customHeight="1">
       <c r="A42" s="45" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="B42" s="46">
-        <v>1250</v>
+        <v>1100</v>
       </c>
       <c r="C42" s="46">
-        <v>1350</v>
+        <v>1190</v>
       </c>
       <c r="D42" s="38"/>
       <c r="E42" s="38"/>
@@ -5098,17 +5101,17 @@
       <c r="L42" s="38"/>
       <c r="M42" s="38"/>
       <c r="N42" s="38"/>
-      <c r="O42" s="75"/>
+      <c r="O42" s="57"/>
     </row>
     <row r="43" spans="1:15" ht="19.5" customHeight="1">
       <c r="A43" s="45" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B43" s="46">
-        <v>1370</v>
+        <v>1250</v>
       </c>
       <c r="C43" s="46">
-        <v>1490</v>
+        <v>1350</v>
       </c>
       <c r="D43" s="38"/>
       <c r="E43" s="38"/>
@@ -5123,12 +5126,18 @@
       <c r="L43" s="38"/>
       <c r="M43" s="38"/>
       <c r="N43" s="38"/>
-      <c r="O43" s="75"/>
+      <c r="O43" s="57"/>
     </row>
     <row r="44" spans="1:15" ht="19.5" customHeight="1">
-      <c r="A44" s="44"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
+      <c r="A44" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="36">
+        <v>1370</v>
+      </c>
+      <c r="C44" s="36">
+        <v>1490</v>
+      </c>
       <c r="D44" s="38"/>
       <c r="E44" s="38"/>
       <c r="F44" s="38"/>
@@ -5142,7 +5151,7 @@
       <c r="L44" s="38"/>
       <c r="M44" s="38"/>
       <c r="N44" s="38"/>
-      <c r="O44" s="75"/>
+      <c r="O44" s="57"/>
     </row>
     <row r="45" spans="1:15" ht="19.5" customHeight="1">
       <c r="A45" s="45"/>
@@ -5161,7 +5170,7 @@
       <c r="L45" s="38"/>
       <c r="M45" s="38"/>
       <c r="N45" s="38"/>
-      <c r="O45" s="75"/>
+      <c r="O45" s="57"/>
     </row>
     <row r="46" spans="1:15" ht="19.5" customHeight="1">
       <c r="A46" s="45"/>
@@ -5180,7 +5189,7 @@
       <c r="L46" s="38"/>
       <c r="M46" s="38"/>
       <c r="N46" s="38"/>
-      <c r="O46" s="75"/>
+      <c r="O46" s="57"/>
     </row>
     <row r="47" spans="1:15" ht="19.5" customHeight="1">
       <c r="A47" s="45"/>
@@ -5199,7 +5208,7 @@
       <c r="L47" s="38"/>
       <c r="M47" s="38"/>
       <c r="N47" s="38"/>
-      <c r="O47" s="75"/>
+      <c r="O47" s="57"/>
     </row>
     <row r="48" spans="1:15" ht="19.5" customHeight="1">
       <c r="A48" s="44"/>
@@ -5218,47 +5227,47 @@
       <c r="L48" s="38"/>
       <c r="M48" s="38"/>
       <c r="N48" s="38"/>
-      <c r="O48" s="76"/>
+      <c r="O48" s="58"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="47" t="s">
+      <c r="A49" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="65"/>
       <c r="D49" s="32"/>
-      <c r="E49" s="51" t="s">
+      <c r="E49" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="F49" s="51"/>
-      <c r="G49" s="51"/>
-      <c r="H49" s="51"/>
-      <c r="I49" s="51"/>
-      <c r="J49" s="51"/>
-      <c r="K49" s="51"/>
+      <c r="F49" s="68"/>
+      <c r="G49" s="68"/>
+      <c r="H49" s="68"/>
+      <c r="I49" s="68"/>
+      <c r="J49" s="68"/>
+      <c r="K49" s="68"/>
       <c r="L49" s="32"/>
-      <c r="M49" s="53" t="s">
+      <c r="M49" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="N49" s="53"/>
-      <c r="O49" s="54"/>
+      <c r="N49" s="70"/>
+      <c r="O49" s="71"/>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A50" s="49"/>
-      <c r="B50" s="50"/>
-      <c r="C50" s="50"/>
+      <c r="A50" s="66"/>
+      <c r="B50" s="67"/>
+      <c r="C50" s="67"/>
       <c r="D50" s="33"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="52"/>
-      <c r="G50" s="52"/>
-      <c r="H50" s="52"/>
-      <c r="I50" s="52"/>
-      <c r="J50" s="52"/>
-      <c r="K50" s="52"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="69"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="69"/>
       <c r="L50" s="33"/>
-      <c r="M50" s="55"/>
-      <c r="N50" s="55"/>
-      <c r="O50" s="56"/>
+      <c r="M50" s="72"/>
+      <c r="N50" s="72"/>
+      <c r="O50" s="73"/>
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="29"/>
@@ -5278,27 +5287,27 @@
       <c r="O51" s="30"/>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="57" t="s">
+      <c r="A52" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
+      <c r="B52" s="74"/>
+      <c r="C52" s="74"/>
       <c r="D52" s="35"/>
       <c r="E52" s="29"/>
       <c r="F52" s="29"/>
-      <c r="G52" s="59" t="s">
+      <c r="G52" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="H52" s="60"/>
-      <c r="I52" s="61"/>
+      <c r="H52" s="77"/>
+      <c r="I52" s="78"/>
       <c r="J52" s="29"/>
       <c r="K52" s="29"/>
       <c r="L52" s="35"/>
-      <c r="M52" s="58" t="s">
+      <c r="M52" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="N52" s="58"/>
-      <c r="O52" s="58"/>
+      <c r="N52" s="75"/>
+      <c r="O52" s="75"/>
     </row>
     <row r="53" spans="1:16">
       <c r="A53" s="34"/>
@@ -5307,9 +5316,9 @@
       <c r="D53" s="35"/>
       <c r="E53" s="29"/>
       <c r="F53" s="29"/>
-      <c r="G53" s="62"/>
-      <c r="H53" s="63"/>
-      <c r="I53" s="64"/>
+      <c r="G53" s="79"/>
+      <c r="H53" s="80"/>
+      <c r="I53" s="81"/>
       <c r="J53" s="29"/>
       <c r="K53" s="29"/>
       <c r="L53" s="35"/>
@@ -5322,6 +5331,18 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A49:C50"/>
+    <mergeCell ref="E49:K50"/>
+    <mergeCell ref="M49:O50"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="M52:O52"/>
+    <mergeCell ref="G52:I53"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:O3"/>
     <mergeCell ref="I36:J36"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="A2:O2"/>
@@ -5329,18 +5350,6 @@
     <mergeCell ref="I38:N38"/>
     <mergeCell ref="O38:O48"/>
     <mergeCell ref="K39:N39"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A49:C50"/>
-    <mergeCell ref="E49:K50"/>
-    <mergeCell ref="M49:O50"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="M52:O52"/>
-    <mergeCell ref="G52:I53"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
@@ -5377,73 +5386,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="89" t="s">
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="87"/>
+      <c r="N2" s="87"/>
+      <c r="O2" s="87"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="82" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5451,12 +5460,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="88" t="s">
+      <c r="L4" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="6" t="s">
@@ -6560,14 +6569,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="81" t="s">
+      <c r="I44" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="82"/>
+      <c r="J44" s="90"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="81"/>
-      <c r="N44" s="81"/>
+      <c r="M44" s="89"/>
+      <c r="N44" s="89"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -6585,13 +6594,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="81"/>
-      <c r="J45" s="81"/>
-      <c r="K45" s="81"/>
-      <c r="L45" s="81"/>
-      <c r="M45" s="81"/>
-      <c r="N45" s="81"/>
-      <c r="O45" s="81"/>
+      <c r="I45" s="89"/>
+      <c r="J45" s="89"/>
+      <c r="K45" s="89"/>
+      <c r="L45" s="89"/>
+      <c r="M45" s="89"/>
+      <c r="N45" s="89"/>
+      <c r="O45" s="89"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="9" t="s">
@@ -6608,15 +6617,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="83" t="s">
+      <c r="I46" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="83"/>
-      <c r="K46" s="83"/>
-      <c r="L46" s="83"/>
-      <c r="M46" s="83"/>
-      <c r="N46" s="83"/>
-      <c r="O46" s="84"/>
+      <c r="J46" s="91"/>
+      <c r="K46" s="91"/>
+      <c r="L46" s="91"/>
+      <c r="M46" s="91"/>
+      <c r="N46" s="91"/>
+      <c r="O46" s="92"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="9" t="s">
@@ -6639,13 +6648,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="81" t="s">
+      <c r="K47" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="81"/>
-      <c r="M47" s="81"/>
-      <c r="N47" s="81"/>
-      <c r="O47" s="85"/>
+      <c r="L47" s="89"/>
+      <c r="M47" s="89"/>
+      <c r="N47" s="89"/>
+      <c r="O47" s="93"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="9" t="s">
@@ -6670,7 +6679,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="85"/>
+      <c r="O48" s="93"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="9" t="s">
@@ -6695,7 +6704,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="85"/>
+      <c r="O49" s="93"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="4" t="s">
@@ -6720,7 +6729,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="85"/>
+      <c r="O50" s="93"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="4" t="s">
@@ -6745,7 +6754,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="85"/>
+      <c r="O51" s="93"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="4" t="s">
@@ -6770,7 +6779,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="85"/>
+      <c r="O52" s="93"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="4" t="s">
@@ -6795,7 +6804,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="85"/>
+      <c r="O53" s="93"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="4" t="s">
@@ -6820,7 +6829,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="85"/>
+      <c r="O54" s="93"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="4" t="s">
@@ -6845,7 +6854,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="85"/>
+      <c r="O55" s="93"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="9" t="s">
@@ -6870,7 +6879,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="86"/>
+      <c r="O56" s="94"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="17"/>
@@ -6890,49 +6899,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="77" t="s">
+      <c r="A58" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="77"/>
-      <c r="C58" s="77"/>
+      <c r="B58" s="95"/>
+      <c r="C58" s="95"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="80" t="s">
+      <c r="F58" s="98" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="80"/>
-      <c r="H58" s="80"/>
-      <c r="I58" s="80"/>
-      <c r="J58" s="80"/>
-      <c r="K58" s="80"/>
+      <c r="G58" s="98"/>
+      <c r="H58" s="98"/>
+      <c r="I58" s="98"/>
+      <c r="J58" s="98"/>
+      <c r="K58" s="98"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="78" t="s">
+      <c r="N58" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="78"/>
+      <c r="O58" s="96"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="79"/>
-      <c r="B59" s="79"/>
-      <c r="C59" s="79"/>
+      <c r="A59" s="97"/>
+      <c r="B59" s="97"/>
+      <c r="C59" s="97"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="80"/>
-      <c r="G59" s="80"/>
-      <c r="H59" s="80"/>
-      <c r="I59" s="80"/>
-      <c r="J59" s="80"/>
-      <c r="K59" s="80"/>
+      <c r="F59" s="98"/>
+      <c r="G59" s="98"/>
+      <c r="H59" s="98"/>
+      <c r="I59" s="98"/>
+      <c r="J59" s="98"/>
+      <c r="K59" s="98"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="79"/>
-      <c r="O59" s="79"/>
+      <c r="N59" s="97"/>
+      <c r="O59" s="97"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="79"/>
-      <c r="B60" s="79"/>
-      <c r="C60" s="79"/>
+      <c r="A60" s="97"/>
+      <c r="B60" s="97"/>
+      <c r="C60" s="97"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -6943,15 +6952,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="79"/>
-      <c r="O60" s="79"/>
+      <c r="N60" s="97"/>
+      <c r="O60" s="97"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="77" t="s">
+      <c r="A61" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="77"/>
-      <c r="C61" s="77"/>
+      <c r="B61" s="95"/>
+      <c r="C61" s="95"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -6962,11 +6971,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="78"/>
-      <c r="O61" s="78"/>
+      <c r="N61" s="96"/>
+      <c r="O61" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="N58:O58"/>
+    <mergeCell ref="A59:C60"/>
+    <mergeCell ref="N59:O60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="N61:O61"/>
+    <mergeCell ref="F58:K59"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="L4:O4"/>
     <mergeCell ref="A1:E1"/>
@@ -6974,19 +6996,6 @@
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="A3:O3"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="N58:O58"/>
-    <mergeCell ref="A59:C60"/>
-    <mergeCell ref="N59:O60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="N61:O61"/>
-    <mergeCell ref="F58:K59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
13.10.19 & 14.10.19 Sales Details
</commit_message>
<xml_diff>
--- a/October/Others/Allocation Sheet.xlsx
+++ b/October/Others/Allocation Sheet.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="123">
   <si>
     <t>BL60</t>
   </si>
@@ -439,7 +439,10 @@
     <t>D40i</t>
   </si>
   <si>
-    <t>Md Shohel Rana</t>
+    <t>i68</t>
+  </si>
+  <si>
+    <t>Md Robiul Islam</t>
   </si>
 </sst>
 </file>
@@ -940,6 +943,81 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -958,74 +1036,35 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1046,42 +1085,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1484,7 +1487,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2584,7 +2587,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3030,7 +3033,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3101,7 +3104,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3175,7 +3178,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3246,7 +3249,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3908,7 +3911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection sqref="A1:O53"/>
     </sheetView>
   </sheetViews>
@@ -3932,65 +3935,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="59" t="s">
+      <c r="A1" s="75"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
+      <c r="O2" s="79"/>
     </row>
     <row r="3" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
       <c r="A3" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="61"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="74"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
-      <c r="K3" s="99" t="s">
+      <c r="K3" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="L3" s="99"/>
-      <c r="M3" s="100" t="s">
-        <v>121</v>
-      </c>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="77" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
     </row>
     <row r="4" spans="1:15" ht="19.5" customHeight="1" thickTop="1">
       <c r="A4" s="50" t="s">
@@ -4198,13 +4201,13 @@
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
       <c r="I10" s="44" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="J10" s="39">
-        <v>5940</v>
+        <v>5550</v>
       </c>
       <c r="K10" s="38">
-        <v>6390</v>
+        <v>5990</v>
       </c>
       <c r="L10" s="38"/>
       <c r="M10" s="38"/>
@@ -4227,13 +4230,13 @@
       <c r="G11" s="38"/>
       <c r="H11" s="38"/>
       <c r="I11" s="43" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="J11" s="39">
-        <v>6530</v>
+        <v>5940</v>
       </c>
       <c r="K11" s="38">
-        <v>6990</v>
+        <v>6390</v>
       </c>
       <c r="L11" s="38"/>
       <c r="M11" s="38"/>
@@ -4256,13 +4259,13 @@
       <c r="G12" s="38"/>
       <c r="H12" s="38"/>
       <c r="I12" s="44" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="J12" s="39">
-        <v>6890</v>
+        <v>6530</v>
       </c>
       <c r="K12" s="38">
-        <v>7490</v>
+        <v>6990</v>
       </c>
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>
@@ -4285,13 +4288,13 @@
       <c r="G13" s="38"/>
       <c r="H13" s="38"/>
       <c r="I13" s="44" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="J13" s="39">
-        <v>8340</v>
+        <v>6890</v>
       </c>
       <c r="K13" s="38">
-        <v>8990</v>
+        <v>7490</v>
       </c>
       <c r="L13" s="38"/>
       <c r="M13" s="38"/>
@@ -4314,13 +4317,13 @@
       <c r="G14" s="38"/>
       <c r="H14" s="38"/>
       <c r="I14" s="44" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="J14" s="39">
-        <v>9190</v>
+        <v>8340</v>
       </c>
       <c r="K14" s="38">
-        <v>9990</v>
+        <v>8990</v>
       </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38"/>
@@ -4343,13 +4346,13 @@
       <c r="G15" s="38"/>
       <c r="H15" s="38"/>
       <c r="I15" s="44" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="J15" s="40">
-        <v>5750</v>
+        <v>9190</v>
       </c>
       <c r="K15" s="46">
-        <v>6190</v>
+        <v>9990</v>
       </c>
       <c r="L15" s="38"/>
       <c r="M15" s="38"/>
@@ -4372,13 +4375,13 @@
       <c r="G16" s="38"/>
       <c r="H16" s="38"/>
       <c r="I16" s="43" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="J16" s="40">
-        <v>3560</v>
+        <v>5750</v>
       </c>
       <c r="K16" s="46">
-        <v>3840</v>
+        <v>6190</v>
       </c>
       <c r="L16" s="38"/>
       <c r="M16" s="38"/>
@@ -4401,13 +4404,13 @@
       <c r="G17" s="38"/>
       <c r="H17" s="38"/>
       <c r="I17" s="44" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="J17" s="40">
-        <v>3340</v>
+        <v>3560</v>
       </c>
       <c r="K17" s="46">
-        <v>3590</v>
+        <v>3840</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="38"/>
@@ -4430,13 +4433,13 @@
       <c r="G18" s="38"/>
       <c r="H18" s="38"/>
       <c r="I18" s="44" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="J18" s="39">
-        <v>4500</v>
+        <v>3340</v>
       </c>
       <c r="K18" s="46">
-        <v>4790</v>
+        <v>3590</v>
       </c>
       <c r="L18" s="38"/>
       <c r="M18" s="38"/>
@@ -4459,13 +4462,13 @@
       <c r="G19" s="38"/>
       <c r="H19" s="38"/>
       <c r="I19" s="43" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="J19" s="39">
-        <v>3710</v>
+        <v>4500</v>
       </c>
       <c r="K19" s="46">
-        <v>3990</v>
+        <v>4790</v>
       </c>
       <c r="L19" s="38"/>
       <c r="M19" s="38"/>
@@ -4488,13 +4491,13 @@
       <c r="G20" s="38"/>
       <c r="H20" s="38"/>
       <c r="I20" s="43" t="s">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="J20" s="39">
-        <v>3620</v>
+        <v>3710</v>
       </c>
       <c r="K20" s="38">
-        <v>3890</v>
+        <v>3990</v>
       </c>
       <c r="L20" s="38"/>
       <c r="M20" s="38"/>
@@ -4517,13 +4520,13 @@
       <c r="G21" s="38"/>
       <c r="H21" s="38"/>
       <c r="I21" s="43" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="J21" s="39">
-        <v>4080</v>
+        <v>3620</v>
       </c>
       <c r="K21" s="38">
-        <v>4390</v>
+        <v>3890</v>
       </c>
       <c r="L21" s="38"/>
       <c r="M21" s="38"/>
@@ -4546,13 +4549,13 @@
       <c r="G22" s="38"/>
       <c r="H22" s="38"/>
       <c r="I22" s="44" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="J22" s="40">
-        <v>4220</v>
+        <v>4080</v>
       </c>
       <c r="K22" s="38">
-        <v>4540</v>
+        <v>4390</v>
       </c>
       <c r="L22" s="38"/>
       <c r="M22" s="38"/>
@@ -4575,13 +4578,13 @@
       <c r="G23" s="38"/>
       <c r="H23" s="38"/>
       <c r="I23" s="43" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="J23" s="40">
-        <v>3710</v>
+        <v>4220</v>
       </c>
       <c r="K23" s="38">
-        <v>3990</v>
+        <v>4540</v>
       </c>
       <c r="L23" s="38"/>
       <c r="M23" s="38"/>
@@ -4604,13 +4607,13 @@
       <c r="G24" s="38"/>
       <c r="H24" s="38"/>
       <c r="I24" s="43" t="s">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="J24" s="40">
-        <v>4280</v>
+        <v>3710</v>
       </c>
       <c r="K24" s="38">
-        <v>4590</v>
+        <v>3990</v>
       </c>
       <c r="L24" s="38"/>
       <c r="M24" s="38"/>
@@ -4633,13 +4636,13 @@
       <c r="G25" s="38"/>
       <c r="H25" s="38"/>
       <c r="I25" s="43" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="J25" s="39">
-        <v>5020</v>
+        <v>4280</v>
       </c>
       <c r="K25" s="38">
-        <v>5390</v>
+        <v>4590</v>
       </c>
       <c r="L25" s="38"/>
       <c r="M25" s="38"/>
@@ -4666,13 +4669,13 @@
       <c r="G26" s="38"/>
       <c r="H26" s="38"/>
       <c r="I26" s="44" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="J26" s="40">
-        <v>5280</v>
+        <v>5020</v>
       </c>
       <c r="K26" s="38">
-        <v>5690</v>
+        <v>5390</v>
       </c>
       <c r="L26" s="38"/>
       <c r="M26" s="38"/>
@@ -4699,13 +4702,13 @@
       <c r="G27" s="38"/>
       <c r="H27" s="38"/>
       <c r="I27" s="44" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="J27" s="39">
-        <v>4550</v>
+        <v>5280</v>
       </c>
       <c r="K27" s="38">
-        <v>4890</v>
+        <v>5690</v>
       </c>
       <c r="L27" s="38"/>
       <c r="M27" s="38"/>
@@ -4732,13 +4735,13 @@
       <c r="G28" s="38"/>
       <c r="H28" s="38"/>
       <c r="I28" s="43" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="J28" s="39">
-        <v>5100</v>
+        <v>4550</v>
       </c>
       <c r="K28" s="38">
-        <v>5490</v>
+        <v>4890</v>
       </c>
       <c r="L28" s="38"/>
       <c r="M28" s="38"/>
@@ -4765,13 +4768,13 @@
       <c r="G29" s="38"/>
       <c r="H29" s="38"/>
       <c r="I29" s="43" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="J29" s="39">
-        <v>5390</v>
+        <v>5100</v>
       </c>
       <c r="K29" s="38">
-        <v>5790</v>
+        <v>5490</v>
       </c>
       <c r="L29" s="38"/>
       <c r="M29" s="38"/>
@@ -4794,13 +4797,13 @@
       <c r="G30" s="38"/>
       <c r="H30" s="38"/>
       <c r="I30" s="43" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="J30" s="39">
-        <v>12090</v>
+        <v>5390</v>
       </c>
       <c r="K30" s="38">
-        <v>12990</v>
+        <v>5790</v>
       </c>
       <c r="L30" s="38"/>
       <c r="M30" s="38"/>
@@ -4811,18 +4814,22 @@
       <c r="A31" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="37"/>
-      <c r="C31" s="46"/>
+      <c r="B31" s="37">
+        <v>970</v>
+      </c>
+      <c r="C31" s="46">
+        <v>1050</v>
+      </c>
       <c r="D31" s="38"/>
       <c r="E31" s="38"/>
       <c r="F31" s="38"/>
       <c r="G31" s="38"/>
       <c r="H31" s="38"/>
       <c r="I31" s="43" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J31" s="39">
-        <v>12240</v>
+        <v>12090</v>
       </c>
       <c r="K31" s="38">
         <v>12990</v>
@@ -4848,13 +4855,13 @@
       <c r="G32" s="38"/>
       <c r="H32" s="38"/>
       <c r="I32" s="45" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="J32" s="40">
-        <v>8820</v>
+        <v>12240</v>
       </c>
       <c r="K32" s="38">
-        <v>9490</v>
+        <v>12990</v>
       </c>
       <c r="L32" s="38"/>
       <c r="M32" s="38"/>
@@ -4876,9 +4883,15 @@
       <c r="F33" s="38"/>
       <c r="G33" s="38"/>
       <c r="H33" s="38"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="38"/>
+      <c r="I33" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="J33" s="39">
+        <v>8820</v>
+      </c>
+      <c r="K33" s="38">
+        <v>9490</v>
+      </c>
       <c r="L33" s="38"/>
       <c r="M33" s="38"/>
       <c r="N33" s="38"/>
@@ -4945,14 +4958,14 @@
       <c r="F36" s="38"/>
       <c r="G36" s="38"/>
       <c r="H36" s="38"/>
-      <c r="I36" s="53" t="s">
+      <c r="I36" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="J36" s="53"/>
+      <c r="J36" s="78"/>
       <c r="K36" s="38"/>
       <c r="L36" s="38"/>
-      <c r="M36" s="53"/>
-      <c r="N36" s="53"/>
+      <c r="M36" s="78"/>
+      <c r="N36" s="78"/>
       <c r="O36" s="41"/>
     </row>
     <row r="37" spans="1:15" ht="19.5" customHeight="1">
@@ -4970,13 +4983,13 @@
       <c r="F37" s="38"/>
       <c r="G37" s="38"/>
       <c r="H37" s="38"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
-      <c r="O37" s="53"/>
+      <c r="I37" s="78"/>
+      <c r="J37" s="78"/>
+      <c r="K37" s="78"/>
+      <c r="L37" s="78"/>
+      <c r="M37" s="78"/>
+      <c r="N37" s="78"/>
+      <c r="O37" s="78"/>
     </row>
     <row r="38" spans="1:15" ht="19.5" customHeight="1">
       <c r="A38" s="45" t="s">
@@ -4993,15 +5006,15 @@
       <c r="F38" s="38"/>
       <c r="G38" s="38"/>
       <c r="H38" s="38"/>
-      <c r="I38" s="55" t="s">
+      <c r="I38" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="55"/>
-      <c r="M38" s="55"/>
-      <c r="N38" s="55"/>
-      <c r="O38" s="56"/>
+      <c r="J38" s="80"/>
+      <c r="K38" s="80"/>
+      <c r="L38" s="80"/>
+      <c r="M38" s="80"/>
+      <c r="N38" s="80"/>
+      <c r="O38" s="81"/>
     </row>
     <row r="39" spans="1:15" ht="19.5" customHeight="1">
       <c r="A39" s="45" t="s">
@@ -5024,13 +5037,13 @@
       <c r="J39" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="K39" s="53" t="s">
+      <c r="K39" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="L39" s="53"/>
-      <c r="M39" s="53"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="57"/>
+      <c r="L39" s="78"/>
+      <c r="M39" s="78"/>
+      <c r="N39" s="78"/>
+      <c r="O39" s="82"/>
     </row>
     <row r="40" spans="1:15" ht="19.5" customHeight="1">
       <c r="A40" s="45" t="s">
@@ -5055,7 +5068,7 @@
       <c r="L40" s="38"/>
       <c r="M40" s="38"/>
       <c r="N40" s="38"/>
-      <c r="O40" s="57"/>
+      <c r="O40" s="82"/>
     </row>
     <row r="41" spans="1:15" ht="19.5" customHeight="1">
       <c r="A41" s="45" t="s">
@@ -5076,7 +5089,7 @@
       <c r="L41" s="38"/>
       <c r="M41" s="38"/>
       <c r="N41" s="38"/>
-      <c r="O41" s="57"/>
+      <c r="O41" s="82"/>
     </row>
     <row r="42" spans="1:15" ht="19.5" customHeight="1">
       <c r="A42" s="45" t="s">
@@ -5101,7 +5114,7 @@
       <c r="L42" s="38"/>
       <c r="M42" s="38"/>
       <c r="N42" s="38"/>
-      <c r="O42" s="57"/>
+      <c r="O42" s="82"/>
     </row>
     <row r="43" spans="1:15" ht="19.5" customHeight="1">
       <c r="A43" s="45" t="s">
@@ -5126,7 +5139,7 @@
       <c r="L43" s="38"/>
       <c r="M43" s="38"/>
       <c r="N43" s="38"/>
-      <c r="O43" s="57"/>
+      <c r="O43" s="82"/>
     </row>
     <row r="44" spans="1:15" ht="19.5" customHeight="1">
       <c r="A44" s="44" t="s">
@@ -5151,7 +5164,7 @@
       <c r="L44" s="38"/>
       <c r="M44" s="38"/>
       <c r="N44" s="38"/>
-      <c r="O44" s="57"/>
+      <c r="O44" s="82"/>
     </row>
     <row r="45" spans="1:15" ht="19.5" customHeight="1">
       <c r="A45" s="45"/>
@@ -5170,7 +5183,7 @@
       <c r="L45" s="38"/>
       <c r="M45" s="38"/>
       <c r="N45" s="38"/>
-      <c r="O45" s="57"/>
+      <c r="O45" s="82"/>
     </row>
     <row r="46" spans="1:15" ht="19.5" customHeight="1">
       <c r="A46" s="45"/>
@@ -5189,7 +5202,7 @@
       <c r="L46" s="38"/>
       <c r="M46" s="38"/>
       <c r="N46" s="38"/>
-      <c r="O46" s="57"/>
+      <c r="O46" s="82"/>
     </row>
     <row r="47" spans="1:15" ht="19.5" customHeight="1">
       <c r="A47" s="45"/>
@@ -5208,7 +5221,7 @@
       <c r="L47" s="38"/>
       <c r="M47" s="38"/>
       <c r="N47" s="38"/>
-      <c r="O47" s="57"/>
+      <c r="O47" s="82"/>
     </row>
     <row r="48" spans="1:15" ht="19.5" customHeight="1">
       <c r="A48" s="44"/>
@@ -5227,47 +5240,47 @@
       <c r="L48" s="38"/>
       <c r="M48" s="38"/>
       <c r="N48" s="38"/>
-      <c r="O48" s="58"/>
+      <c r="O48" s="83"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="64" t="s">
+      <c r="A49" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="B49" s="65"/>
-      <c r="C49" s="65"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="54"/>
       <c r="D49" s="32"/>
-      <c r="E49" s="68" t="s">
+      <c r="E49" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="F49" s="68"/>
-      <c r="G49" s="68"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="68"/>
-      <c r="J49" s="68"/>
-      <c r="K49" s="68"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="57"/>
+      <c r="J49" s="57"/>
+      <c r="K49" s="57"/>
       <c r="L49" s="32"/>
-      <c r="M49" s="70" t="s">
+      <c r="M49" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="N49" s="70"/>
-      <c r="O49" s="71"/>
+      <c r="N49" s="59"/>
+      <c r="O49" s="60"/>
     </row>
     <row r="50" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A50" s="66"/>
-      <c r="B50" s="67"/>
-      <c r="C50" s="67"/>
+      <c r="A50" s="55"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="56"/>
       <c r="D50" s="33"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="69"/>
-      <c r="H50" s="69"/>
-      <c r="I50" s="69"/>
-      <c r="J50" s="69"/>
-      <c r="K50" s="69"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="58"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="58"/>
+      <c r="J50" s="58"/>
+      <c r="K50" s="58"/>
       <c r="L50" s="33"/>
-      <c r="M50" s="72"/>
-      <c r="N50" s="72"/>
-      <c r="O50" s="73"/>
+      <c r="M50" s="61"/>
+      <c r="N50" s="61"/>
+      <c r="O50" s="62"/>
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="29"/>
@@ -5287,27 +5300,27 @@
       <c r="O51" s="30"/>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="74" t="s">
+      <c r="A52" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="74"/>
-      <c r="C52" s="74"/>
+      <c r="B52" s="63"/>
+      <c r="C52" s="63"/>
       <c r="D52" s="35"/>
       <c r="E52" s="29"/>
       <c r="F52" s="29"/>
-      <c r="G52" s="76" t="s">
+      <c r="G52" s="65" t="s">
         <v>114</v>
       </c>
-      <c r="H52" s="77"/>
-      <c r="I52" s="78"/>
+      <c r="H52" s="66"/>
+      <c r="I52" s="67"/>
       <c r="J52" s="29"/>
       <c r="K52" s="29"/>
       <c r="L52" s="35"/>
-      <c r="M52" s="75" t="s">
+      <c r="M52" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="N52" s="75"/>
-      <c r="O52" s="75"/>
+      <c r="N52" s="64"/>
+      <c r="O52" s="64"/>
     </row>
     <row r="53" spans="1:16">
       <c r="A53" s="34"/>
@@ -5316,9 +5329,9 @@
       <c r="D53" s="35"/>
       <c r="E53" s="29"/>
       <c r="F53" s="29"/>
-      <c r="G53" s="79"/>
-      <c r="H53" s="80"/>
-      <c r="I53" s="81"/>
+      <c r="G53" s="68"/>
+      <c r="H53" s="69"/>
+      <c r="I53" s="70"/>
       <c r="J53" s="29"/>
       <c r="K53" s="29"/>
       <c r="L53" s="35"/>
@@ -5331,18 +5344,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A49:C50"/>
-    <mergeCell ref="E49:K50"/>
-    <mergeCell ref="M49:O50"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="M52:O52"/>
-    <mergeCell ref="G52:I53"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="M3:O3"/>
     <mergeCell ref="I36:J36"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="A2:O2"/>
@@ -5350,6 +5351,18 @@
     <mergeCell ref="I38:N38"/>
     <mergeCell ref="O38:O48"/>
     <mergeCell ref="K39:N39"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="A49:C50"/>
+    <mergeCell ref="E49:K50"/>
+    <mergeCell ref="M49:O50"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="M52:O52"/>
+    <mergeCell ref="G52:I53"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.2" header="0" footer="0"/>
@@ -5386,73 +5399,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="32.25" customHeight="1">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="96" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="86" t="s">
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="98" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="84" t="s">
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="96" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="87"/>
-      <c r="O2" s="87"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="88"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
     </row>
     <row r="4" spans="1:15" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5460,12 +5473,12 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="83" t="s">
+      <c r="L4" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="83"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="95"/>
     </row>
     <row r="5" spans="1:15" ht="16.5" thickTop="1">
       <c r="A5" s="6" t="s">
@@ -6569,14 +6582,14 @@
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="89" t="s">
+      <c r="I44" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="J44" s="90"/>
+      <c r="J44" s="89"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
-      <c r="M44" s="89"/>
-      <c r="N44" s="89"/>
+      <c r="M44" s="88"/>
+      <c r="N44" s="88"/>
       <c r="O44" s="16"/>
     </row>
     <row r="45" spans="1:15" ht="15.95" customHeight="1">
@@ -6594,13 +6607,13 @@
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-      <c r="I45" s="89"/>
-      <c r="J45" s="89"/>
-      <c r="K45" s="89"/>
-      <c r="L45" s="89"/>
-      <c r="M45" s="89"/>
-      <c r="N45" s="89"/>
-      <c r="O45" s="89"/>
+      <c r="I45" s="88"/>
+      <c r="J45" s="88"/>
+      <c r="K45" s="88"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="88"/>
+      <c r="N45" s="88"/>
+      <c r="O45" s="88"/>
     </row>
     <row r="46" spans="1:15" ht="15.95" customHeight="1">
       <c r="A46" s="9" t="s">
@@ -6617,15 +6630,15 @@
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
-      <c r="I46" s="91" t="s">
+      <c r="I46" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="91"/>
-      <c r="K46" s="91"/>
-      <c r="L46" s="91"/>
-      <c r="M46" s="91"/>
-      <c r="N46" s="91"/>
-      <c r="O46" s="92"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
+      <c r="L46" s="90"/>
+      <c r="M46" s="90"/>
+      <c r="N46" s="90"/>
+      <c r="O46" s="91"/>
     </row>
     <row r="47" spans="1:15" ht="15.95" customHeight="1">
       <c r="A47" s="9" t="s">
@@ -6648,13 +6661,13 @@
       <c r="J47" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K47" s="89" t="s">
+      <c r="K47" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="L47" s="89"/>
-      <c r="M47" s="89"/>
-      <c r="N47" s="89"/>
-      <c r="O47" s="93"/>
+      <c r="L47" s="88"/>
+      <c r="M47" s="88"/>
+      <c r="N47" s="88"/>
+      <c r="O47" s="92"/>
     </row>
     <row r="48" spans="1:15" ht="15.95" customHeight="1">
       <c r="A48" s="9" t="s">
@@ -6679,7 +6692,7 @@
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
-      <c r="O48" s="93"/>
+      <c r="O48" s="92"/>
     </row>
     <row r="49" spans="1:15" ht="15.95" customHeight="1">
       <c r="A49" s="9" t="s">
@@ -6704,7 +6717,7 @@
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="93"/>
+      <c r="O49" s="92"/>
     </row>
     <row r="50" spans="1:15" ht="15.95" customHeight="1">
       <c r="A50" s="4" t="s">
@@ -6729,7 +6742,7 @@
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="93"/>
+      <c r="O50" s="92"/>
     </row>
     <row r="51" spans="1:15" ht="15.95" customHeight="1">
       <c r="A51" s="4" t="s">
@@ -6754,7 +6767,7 @@
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
-      <c r="O51" s="93"/>
+      <c r="O51" s="92"/>
     </row>
     <row r="52" spans="1:15" ht="15.95" customHeight="1">
       <c r="A52" s="4" t="s">
@@ -6779,7 +6792,7 @@
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="93"/>
+      <c r="O52" s="92"/>
     </row>
     <row r="53" spans="1:15" ht="15.95" customHeight="1">
       <c r="A53" s="4" t="s">
@@ -6804,7 +6817,7 @@
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="93"/>
+      <c r="O53" s="92"/>
     </row>
     <row r="54" spans="1:15" ht="15.95" customHeight="1">
       <c r="A54" s="4" t="s">
@@ -6829,7 +6842,7 @@
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="93"/>
+      <c r="O54" s="92"/>
     </row>
     <row r="55" spans="1:15" ht="15.95" customHeight="1">
       <c r="A55" s="4" t="s">
@@ -6854,7 +6867,7 @@
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="93"/>
+      <c r="O55" s="92"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1">
       <c r="A56" s="9" t="s">
@@ -6879,7 +6892,7 @@
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="94"/>
+      <c r="O56" s="93"/>
     </row>
     <row r="57" spans="1:15">
       <c r="A57" s="17"/>
@@ -6899,49 +6912,49 @@
       <c r="O57" s="20"/>
     </row>
     <row r="58" spans="1:15">
-      <c r="A58" s="95" t="s">
+      <c r="A58" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="95"/>
-      <c r="C58" s="95"/>
+      <c r="B58" s="84"/>
+      <c r="C58" s="84"/>
       <c r="D58" s="21"/>
       <c r="E58" s="22"/>
-      <c r="F58" s="98" t="s">
+      <c r="F58" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="G58" s="98"/>
-      <c r="H58" s="98"/>
-      <c r="I58" s="98"/>
-      <c r="J58" s="98"/>
-      <c r="K58" s="98"/>
+      <c r="G58" s="87"/>
+      <c r="H58" s="87"/>
+      <c r="I58" s="87"/>
+      <c r="J58" s="87"/>
+      <c r="K58" s="87"/>
       <c r="L58" s="21"/>
       <c r="M58" s="22"/>
-      <c r="N58" s="96" t="s">
+      <c r="N58" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="O58" s="96"/>
+      <c r="O58" s="85"/>
     </row>
     <row r="59" spans="1:15">
-      <c r="A59" s="97"/>
-      <c r="B59" s="97"/>
-      <c r="C59" s="97"/>
+      <c r="A59" s="86"/>
+      <c r="B59" s="86"/>
+      <c r="C59" s="86"/>
       <c r="D59" s="23"/>
       <c r="E59" s="17"/>
-      <c r="F59" s="98"/>
-      <c r="G59" s="98"/>
-      <c r="H59" s="98"/>
-      <c r="I59" s="98"/>
-      <c r="J59" s="98"/>
-      <c r="K59" s="98"/>
+      <c r="F59" s="87"/>
+      <c r="G59" s="87"/>
+      <c r="H59" s="87"/>
+      <c r="I59" s="87"/>
+      <c r="J59" s="87"/>
+      <c r="K59" s="87"/>
       <c r="L59" s="23"/>
       <c r="M59" s="17"/>
-      <c r="N59" s="97"/>
-      <c r="O59" s="97"/>
+      <c r="N59" s="86"/>
+      <c r="O59" s="86"/>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="97"/>
-      <c r="B60" s="97"/>
-      <c r="C60" s="97"/>
+      <c r="A60" s="86"/>
+      <c r="B60" s="86"/>
+      <c r="C60" s="86"/>
       <c r="D60" s="23"/>
       <c r="E60" s="17"/>
       <c r="F60" s="17"/>
@@ -6952,15 +6965,15 @@
       <c r="K60" s="23"/>
       <c r="L60" s="23"/>
       <c r="M60" s="17"/>
-      <c r="N60" s="97"/>
-      <c r="O60" s="97"/>
+      <c r="N60" s="86"/>
+      <c r="O60" s="86"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="95" t="s">
+      <c r="A61" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="95"/>
-      <c r="C61" s="95"/>
+      <c r="B61" s="84"/>
+      <c r="C61" s="84"/>
       <c r="D61" s="21"/>
       <c r="E61" s="21"/>
       <c r="F61" s="21"/>
@@ -6971,11 +6984,24 @@
       <c r="K61" s="21"/>
       <c r="L61" s="21"/>
       <c r="M61" s="25"/>
-      <c r="N61" s="96"/>
-      <c r="O61" s="96"/>
+      <c r="N61" s="85"/>
+      <c r="O61" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I46:N46"/>
+    <mergeCell ref="O46:O56"/>
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="N58:O58"/>
     <mergeCell ref="A59:C60"/>
@@ -6983,19 +7009,6 @@
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="N61:O61"/>
     <mergeCell ref="F58:K59"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I46:N46"/>
-    <mergeCell ref="O46:O56"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
22.10.19 To 24.10.19 Sales Detail
</commit_message>
<xml_diff>
--- a/October/Others/Allocation Sheet.xlsx
+++ b/October/Others/Allocation Sheet.xlsx
@@ -442,7 +442,7 @@
     <t>i68</t>
   </si>
   <si>
-    <t>Md Robiul Islam</t>
+    <t>Md Shohel Rana</t>
   </si>
 </sst>
 </file>
@@ -3911,8 +3911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection sqref="A1:O53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O53" sqref="A1:O53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4887,10 +4887,10 @@
         <v>82</v>
       </c>
       <c r="J33" s="39">
-        <v>8820</v>
+        <v>7890</v>
       </c>
       <c r="K33" s="38">
-        <v>9490</v>
+        <v>8490</v>
       </c>
       <c r="L33" s="38"/>
       <c r="M33" s="38"/>

</xml_diff>